<commit_message>
Now showing all valid products instead of returning empty array.
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasosterle/Documents/code/WEB/react-cintamani/cintamani-next/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oesiw\Documents\code\cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2160" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2160" windowWidth="23040" windowHeight="9645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -1833,9 +1833,6 @@
     <t>TBT005.JPG, TBT003.JPG</t>
   </si>
   <si>
-    <t>w Bodhisattvas - Grüne Tara (Syamatara)</t>
-  </si>
-  <si>
     <t>w Bodhisattvas - Weiße Tara (Sitatara)</t>
   </si>
   <si>
@@ -1846,6 +1843,9 @@
   </si>
   <si>
     <t>MBAva014.JPG, MBAva015.JPG, MBAva016.JPG, MBAva017.JPG, MBAva019.JPG</t>
+  </si>
+  <si>
+    <t>w Bodhisattvas - Gruene Tara (Syamatara)</t>
   </si>
 </sst>
 </file>
@@ -2715,17 +2715,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.1640625" customWidth="1"/>
-    <col min="3" max="3" width="48.83203125" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>371</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5048,7 +5048,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6100,13 +6100,13 @@
         <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G148" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6405,7 +6405,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6842,12 +6842,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C182" t="s">
         <v>265</v>
@@ -6865,12 +6865,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C183" t="s">
         <v>274</v>
@@ -6888,12 +6888,12 @@
         <v>274</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C184" t="s">
         <v>263</v>
@@ -6911,12 +6911,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C185" t="s">
         <v>273</v>
@@ -6934,12 +6934,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C186" t="s">
         <v>272</v>
@@ -6957,12 +6957,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C187" t="s">
         <v>272</v>
@@ -6980,12 +6980,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C188" t="s">
         <v>264</v>
@@ -7003,12 +7003,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C189" t="s">
         <v>268</v>
@@ -7026,12 +7026,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C190" t="s">
         <v>267</v>
@@ -7049,12 +7049,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C191" t="s">
         <v>262</v>
@@ -7072,12 +7072,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C192" t="s">
         <v>269</v>
@@ -7095,12 +7095,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C193" t="s">
         <v>283</v>
@@ -7118,12 +7118,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C194" t="s">
         <v>281</v>
@@ -7141,12 +7141,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C195" t="s">
         <v>282</v>
@@ -7164,12 +7164,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C196" t="s">
         <v>278</v>
@@ -7187,12 +7187,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C197" t="s">
         <v>285</v>
@@ -7210,12 +7210,12 @@
         <v>285</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C198" t="s">
         <v>286</v>
@@ -7233,12 +7233,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C199" t="s">
         <v>280</v>
@@ -7256,12 +7256,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C200" t="s">
         <v>276</v>
@@ -7279,12 +7279,12 @@
         <v>275</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C201" t="s">
         <v>284</v>
@@ -7302,12 +7302,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C202" t="s">
         <v>288</v>
@@ -7325,12 +7325,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C203" t="s">
         <v>290</v>
@@ -7348,7 +7348,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7578,12 +7578,12 @@
         <v>310</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C214" t="s">
         <v>314</v>
@@ -7601,12 +7601,12 @@
         <v>314</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C215" t="s">
         <v>313</v>
@@ -7624,12 +7624,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C216" t="s">
         <v>315</v>
@@ -7647,12 +7647,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C217" t="s">
         <v>312</v>
@@ -7670,7 +7670,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -8153,7 +8153,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>94</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>1</v>
       </c>
       <c r="F240" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G240" t="s">
         <v>134</v>
@@ -8215,9 +8215,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
Adding descriptions for categories, added gruene tara, added PaymentInfo
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oesiw\Documents\code\cintamani\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasosterle/Documents/code/WEB/react-cintamani/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D9A39D-235B-5149-B3A6-C9649DB72AAB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -1805,9 +1806,6 @@
     <t>TBT005.JPG, TBT003.JPG</t>
   </si>
   <si>
-    <t>w Bodhisattvas - Grüne Tara (Syamatara)</t>
-  </si>
-  <si>
     <t>w Bodhisattvas - Weiße Tara (Sitatara)</t>
   </si>
   <si>
@@ -1839,6 +1837,9 @@
   </si>
   <si>
     <t>KKS001.JPG</t>
+  </si>
+  <si>
+    <t>w Bodhisattvas - Gruene Tara (Syamatara)</t>
   </si>
 </sst>
 </file>
@@ -2708,18 +2709,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="6" max="6" width="65.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="6" max="6" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>369</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2788,7 +2789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2834,7 +2835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2926,7 +2927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3156,7 +3157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3179,7 +3180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3248,7 +3249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3271,7 +3272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3340,7 +3341,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3386,7 +3387,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3524,7 +3525,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3547,7 +3548,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3570,7 +3571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3593,7 +3594,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3616,7 +3617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3662,7 +3663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3708,7 +3709,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3754,7 +3755,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3777,7 +3778,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3800,7 +3801,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3823,7 +3824,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3846,7 +3847,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3869,7 +3870,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3915,7 +3916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3938,7 +3939,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3961,7 +3962,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3984,7 +3985,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4030,7 +4031,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4053,7 +4054,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4076,7 +4077,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4099,7 +4100,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4122,7 +4123,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4168,7 +4169,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4191,7 +4192,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4214,7 +4215,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>66</v>
       </c>
@@ -4237,7 +4238,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>67</v>
       </c>
@@ -4260,7 +4261,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>68</v>
       </c>
@@ -4283,7 +4284,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>69</v>
       </c>
@@ -4306,7 +4307,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>70</v>
       </c>
@@ -4323,13 +4324,13 @@
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G70" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>71</v>
       </c>
@@ -4346,13 +4347,13 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G71" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>72</v>
       </c>
@@ -4369,13 +4370,13 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G72" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>73</v>
       </c>
@@ -4392,13 +4393,13 @@
         <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G73" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4415,13 +4416,13 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G74" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>75</v>
       </c>
@@ -4438,13 +4439,13 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G75" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>76</v>
       </c>
@@ -4461,13 +4462,13 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G76" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>77</v>
       </c>
@@ -4484,13 +4485,13 @@
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G77" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>78</v>
       </c>
@@ -4507,13 +4508,13 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G78" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>79</v>
       </c>
@@ -4530,13 +4531,13 @@
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G79" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>80</v>
       </c>
@@ -4553,13 +4554,13 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G80" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>81</v>
       </c>
@@ -4582,7 +4583,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>82</v>
       </c>
@@ -4605,7 +4606,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>83</v>
       </c>
@@ -4628,7 +4629,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>84</v>
       </c>
@@ -4651,7 +4652,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>85</v>
       </c>
@@ -4674,7 +4675,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>86</v>
       </c>
@@ -4697,7 +4698,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>87</v>
       </c>
@@ -4720,7 +4721,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>88</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>89</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>90</v>
       </c>
@@ -4789,7 +4790,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>91</v>
       </c>
@@ -4812,7 +4813,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>92</v>
       </c>
@@ -4835,7 +4836,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>93</v>
       </c>
@@ -4858,7 +4859,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>95</v>
       </c>
@@ -4881,7 +4882,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>96</v>
       </c>
@@ -4904,7 +4905,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>97</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>98</v>
       </c>
@@ -4950,7 +4951,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>99</v>
       </c>
@@ -4973,7 +4974,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>100</v>
       </c>
@@ -4996,7 +4997,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>101</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>102</v>
       </c>
@@ -5042,7 +5043,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>103</v>
       </c>
@@ -5065,7 +5066,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>104</v>
       </c>
@@ -5088,7 +5089,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>105</v>
       </c>
@@ -5111,7 +5112,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>106</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>107</v>
       </c>
@@ -5157,7 +5158,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>108</v>
       </c>
@@ -5180,7 +5181,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>109</v>
       </c>
@@ -5203,7 +5204,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>110</v>
       </c>
@@ -5226,7 +5227,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>111</v>
       </c>
@@ -5249,7 +5250,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>112</v>
       </c>
@@ -5272,7 +5273,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>113</v>
       </c>
@@ -5295,7 +5296,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>114</v>
       </c>
@@ -5318,7 +5319,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>115</v>
       </c>
@@ -5341,7 +5342,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5364,7 +5365,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>117</v>
       </c>
@@ -5387,7 +5388,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>118</v>
       </c>
@@ -5410,7 +5411,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>119</v>
       </c>
@@ -5433,7 +5434,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>120</v>
       </c>
@@ -5456,7 +5457,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>121</v>
       </c>
@@ -5479,7 +5480,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>122</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>123</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>124</v>
       </c>
@@ -5548,7 +5549,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>125</v>
       </c>
@@ -5571,7 +5572,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>126</v>
       </c>
@@ -5594,7 +5595,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>127</v>
       </c>
@@ -5617,7 +5618,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>128</v>
       </c>
@@ -5640,7 +5641,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>129</v>
       </c>
@@ -5663,7 +5664,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>130</v>
       </c>
@@ -5686,7 +5687,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>131</v>
       </c>
@@ -5709,7 +5710,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>132</v>
       </c>
@@ -5732,7 +5733,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>133</v>
       </c>
@@ -5755,7 +5756,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>134</v>
       </c>
@@ -5778,7 +5779,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>135</v>
       </c>
@@ -5801,7 +5802,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>136</v>
       </c>
@@ -5824,7 +5825,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>137</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>138</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>139</v>
       </c>
@@ -5893,7 +5894,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>140</v>
       </c>
@@ -5916,7 +5917,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>141</v>
       </c>
@@ -5939,7 +5940,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>142</v>
       </c>
@@ -5962,7 +5963,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>143</v>
       </c>
@@ -5985,7 +5986,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>144</v>
       </c>
@@ -6008,7 +6009,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>145</v>
       </c>
@@ -6031,7 +6032,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>146</v>
       </c>
@@ -6054,7 +6055,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>147</v>
       </c>
@@ -6071,13 +6072,13 @@
         <v>1</v>
       </c>
       <c r="F147" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G147" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>148</v>
       </c>
@@ -6100,7 +6101,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>149</v>
       </c>
@@ -6123,7 +6124,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>150</v>
       </c>
@@ -6146,7 +6147,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>151</v>
       </c>
@@ -6169,7 +6170,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>152</v>
       </c>
@@ -6192,7 +6193,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>153</v>
       </c>
@@ -6215,7 +6216,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>154</v>
       </c>
@@ -6238,7 +6239,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>155</v>
       </c>
@@ -6261,7 +6262,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>156</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>157</v>
       </c>
@@ -6307,7 +6308,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>158</v>
       </c>
@@ -6330,7 +6331,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>159</v>
       </c>
@@ -6353,7 +6354,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>160</v>
       </c>
@@ -6376,7 +6377,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>161</v>
       </c>
@@ -6399,7 +6400,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>162</v>
       </c>
@@ -6422,7 +6423,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>163</v>
       </c>
@@ -6445,7 +6446,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>164</v>
       </c>
@@ -6468,7 +6469,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>165</v>
       </c>
@@ -6491,7 +6492,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>166</v>
       </c>
@@ -6514,7 +6515,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>167</v>
       </c>
@@ -6537,7 +6538,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>168</v>
       </c>
@@ -6560,7 +6561,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>169</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>170</v>
       </c>
@@ -6606,7 +6607,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>171</v>
       </c>
@@ -6629,7 +6630,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>172</v>
       </c>
@@ -6652,7 +6653,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>173</v>
       </c>
@@ -6675,7 +6676,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>174</v>
       </c>
@@ -6698,7 +6699,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>175</v>
       </c>
@@ -6721,7 +6722,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>176</v>
       </c>
@@ -6744,7 +6745,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>178</v>
       </c>
@@ -6767,7 +6768,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>179</v>
       </c>
@@ -6790,12 +6791,12 @@
         <v>361</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C180" t="s">
         <v>268</v>
@@ -6813,12 +6814,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C181" t="s">
         <v>263</v>
@@ -6836,12 +6837,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>182</v>
       </c>
       <c r="B182" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C182" t="s">
         <v>272</v>
@@ -6859,12 +6860,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>183</v>
       </c>
       <c r="B183" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C183" t="s">
         <v>261</v>
@@ -6882,12 +6883,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>184</v>
       </c>
       <c r="B184" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C184" t="s">
         <v>271</v>
@@ -6905,12 +6906,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>185</v>
       </c>
       <c r="B185" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C185" t="s">
         <v>270</v>
@@ -6928,12 +6929,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>186</v>
       </c>
       <c r="B186" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C186" t="s">
         <v>270</v>
@@ -6951,12 +6952,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>187</v>
       </c>
       <c r="B187" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C187" t="s">
         <v>262</v>
@@ -6974,12 +6975,12 @@
         <v>262</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>188</v>
       </c>
       <c r="B188" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C188" t="s">
         <v>266</v>
@@ -6997,12 +6998,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>189</v>
       </c>
       <c r="B189" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C189" t="s">
         <v>265</v>
@@ -7020,12 +7021,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>190</v>
       </c>
       <c r="B190" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C190" t="s">
         <v>260</v>
@@ -7043,12 +7044,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>191</v>
       </c>
       <c r="B191" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="C191" t="s">
         <v>267</v>
@@ -7066,12 +7067,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>192</v>
       </c>
       <c r="B192" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C192" t="s">
         <v>281</v>
@@ -7089,12 +7090,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>193</v>
       </c>
       <c r="B193" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C193" t="s">
         <v>279</v>
@@ -7112,12 +7113,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>194</v>
       </c>
       <c r="B194" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C194" t="s">
         <v>280</v>
@@ -7135,12 +7136,12 @@
         <v>280</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>195</v>
       </c>
       <c r="B195" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C195" t="s">
         <v>276</v>
@@ -7158,12 +7159,12 @@
         <v>275</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>196</v>
       </c>
       <c r="B196" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C196" t="s">
         <v>283</v>
@@ -7181,12 +7182,12 @@
         <v>283</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>197</v>
       </c>
       <c r="B197" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C197" t="s">
         <v>284</v>
@@ -7204,12 +7205,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>198</v>
       </c>
       <c r="B198" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C198" t="s">
         <v>278</v>
@@ -7227,12 +7228,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>199</v>
       </c>
       <c r="B199" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C199" t="s">
         <v>274</v>
@@ -7250,12 +7251,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>200</v>
       </c>
       <c r="B200" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C200" t="s">
         <v>282</v>
@@ -7273,12 +7274,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>201</v>
       </c>
       <c r="B201" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C201" t="s">
         <v>286</v>
@@ -7296,12 +7297,12 @@
         <v>285</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>202</v>
       </c>
       <c r="B202" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C202" t="s">
         <v>288</v>
@@ -7319,7 +7320,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>203</v>
       </c>
@@ -7342,7 +7343,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>204</v>
       </c>
@@ -7365,7 +7366,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>205</v>
       </c>
@@ -7388,7 +7389,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>206</v>
       </c>
@@ -7411,7 +7412,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>207</v>
       </c>
@@ -7434,7 +7435,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>208</v>
       </c>
@@ -7457,7 +7458,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>209</v>
       </c>
@@ -7480,7 +7481,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>210</v>
       </c>
@@ -7503,7 +7504,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>211</v>
       </c>
@@ -7526,7 +7527,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>212</v>
       </c>
@@ -7549,12 +7550,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>213</v>
       </c>
       <c r="B213" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C213" t="s">
         <v>312</v>
@@ -7572,12 +7573,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>214</v>
       </c>
       <c r="B214" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C214" t="s">
         <v>311</v>
@@ -7595,12 +7596,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>215</v>
       </c>
       <c r="B215" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C215" t="s">
         <v>313</v>
@@ -7618,12 +7619,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>216</v>
       </c>
       <c r="B216" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C216" t="s">
         <v>310</v>
@@ -7641,7 +7642,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>217</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>218</v>
       </c>
@@ -7687,7 +7688,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>219</v>
       </c>
@@ -7710,7 +7711,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>220</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>221</v>
       </c>
@@ -7756,7 +7757,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>222</v>
       </c>
@@ -7779,7 +7780,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>223</v>
       </c>
@@ -7802,7 +7803,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>224</v>
       </c>
@@ -7825,7 +7826,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>225</v>
       </c>
@@ -7848,7 +7849,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>226</v>
       </c>
@@ -7871,7 +7872,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>227</v>
       </c>
@@ -7894,7 +7895,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>228</v>
       </c>
@@ -7917,7 +7918,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>229</v>
       </c>
@@ -7940,7 +7941,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>230</v>
       </c>
@@ -7963,7 +7964,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>231</v>
       </c>
@@ -7986,7 +7987,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>232</v>
       </c>
@@ -8009,7 +8010,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>233</v>
       </c>
@@ -8032,7 +8033,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>234</v>
       </c>
@@ -8055,7 +8056,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>235</v>
       </c>
@@ -8078,7 +8079,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>236</v>
       </c>
@@ -8101,7 +8102,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>237</v>
       </c>
@@ -8124,7 +8125,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>238</v>
       </c>
@@ -8147,7 +8148,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>94</v>
       </c>
@@ -8164,7 +8165,7 @@
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G239" t="s">
         <v>132</v>
@@ -8186,9 +8187,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
Bestellung per Email ermöglicht.
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasosterle/Documents/code/WEB/react-cintamani/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FEEB58-B626-B149-B3D3-49247FEB9372}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDCA10F-C16C-5F47-8165-4E6898526BD8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2080" yWindow="680" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2709,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C243" sqref="C243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
First draft of mobile Menu and updated NEXT
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\code\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2795B2C4-0B6B-476B-8944-3D64AB9331FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2076" yWindow="684" windowWidth="23040" windowHeight="9636"/>
+    <workbookView xWindow="2078" yWindow="683" windowWidth="23040" windowHeight="9638" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -1819,7 +1820,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
@@ -2676,21 +2677,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195:XFD195"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.1328125" customWidth="1"/>
     <col min="3" max="3" width="48.6640625" customWidth="1"/>
     <col min="6" max="6" width="65.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>355</v>
       </c>
@@ -2713,7 +2714,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2851,7 +2852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3012,7 +3013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3081,7 +3082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3219,7 +3220,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3242,7 +3243,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3311,7 +3312,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3334,7 +3335,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3403,7 +3404,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3449,7 +3450,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3472,7 +3473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3495,7 +3496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3518,7 +3519,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3564,7 +3565,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3610,7 +3611,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3633,7 +3634,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3656,7 +3657,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3679,7 +3680,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3748,7 +3749,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3771,7 +3772,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>48</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>49</v>
       </c>
@@ -3817,7 +3818,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="399" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>241</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3886,7 +3887,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3909,7 +3910,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3955,7 +3956,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3978,7 +3979,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4001,7 +4002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4024,7 +4025,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4047,7 +4048,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4070,7 +4071,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4093,7 +4094,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4139,7 +4140,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="399" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>240</v>
       </c>
@@ -4185,7 +4186,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4208,7 +4209,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4231,7 +4232,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4277,7 +4278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4300,7 +4301,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4323,7 +4324,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4369,7 +4370,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4392,7 +4393,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4415,7 +4416,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4438,7 +4439,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4461,7 +4462,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4484,7 +4485,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4507,7 +4508,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4530,7 +4531,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4553,7 +4554,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4576,7 +4577,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4645,7 +4646,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4668,7 +4669,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4691,7 +4692,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4714,7 +4715,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4737,7 +4738,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4760,7 +4761,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>91</v>
       </c>
@@ -4783,7 +4784,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>93</v>
       </c>
@@ -4806,7 +4807,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>95</v>
       </c>
@@ -4829,7 +4830,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>96</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>97</v>
       </c>
@@ -4875,7 +4876,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>98</v>
       </c>
@@ -4898,7 +4899,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>99</v>
       </c>
@@ -4921,7 +4922,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>100</v>
       </c>
@@ -4944,7 +4945,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>101</v>
       </c>
@@ -4967,7 +4968,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>103</v>
       </c>
@@ -4994,7 +4995,7 @@
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>104</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>105</v>
       </c>
@@ -5040,7 +5041,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>106</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>107</v>
       </c>
@@ -5086,7 +5087,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>108</v>
       </c>
@@ -5109,7 +5110,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>109</v>
       </c>
@@ -5132,7 +5133,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>110</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>111</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>112</v>
       </c>
@@ -5201,7 +5202,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>113</v>
       </c>
@@ -5224,7 +5225,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>114</v>
       </c>
@@ -5247,7 +5248,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>115</v>
       </c>
@@ -5270,7 +5271,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>116</v>
       </c>
@@ -5293,7 +5294,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>117</v>
       </c>
@@ -5316,7 +5317,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>118</v>
       </c>
@@ -5339,7 +5340,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>119</v>
       </c>
@@ -5362,7 +5363,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>120</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>121</v>
       </c>
@@ -5408,7 +5409,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>122</v>
       </c>
@@ -5431,7 +5432,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>123</v>
       </c>
@@ -5454,7 +5455,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>124</v>
       </c>
@@ -5477,7 +5478,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>125</v>
       </c>
@@ -5500,7 +5501,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>126</v>
       </c>
@@ -5523,7 +5524,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>127</v>
       </c>
@@ -5546,7 +5547,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>128</v>
       </c>
@@ -5569,7 +5570,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>129</v>
       </c>
@@ -5592,7 +5593,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>130</v>
       </c>
@@ -5615,7 +5616,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>131</v>
       </c>
@@ -5638,7 +5639,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>132</v>
       </c>
@@ -5661,7 +5662,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>133</v>
       </c>
@@ -5684,7 +5685,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>134</v>
       </c>
@@ -5707,7 +5708,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>135</v>
       </c>
@@ -5730,7 +5731,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>136</v>
       </c>
@@ -5753,7 +5754,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>137</v>
       </c>
@@ -5776,7 +5777,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>138</v>
       </c>
@@ -5799,7 +5800,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>139</v>
       </c>
@@ -5822,7 +5823,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>140</v>
       </c>
@@ -5845,7 +5846,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>141</v>
       </c>
@@ -5868,7 +5869,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>142</v>
       </c>
@@ -5891,7 +5892,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>143</v>
       </c>
@@ -5914,7 +5915,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>144</v>
       </c>
@@ -5937,7 +5938,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>145</v>
       </c>
@@ -5960,7 +5961,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>146</v>
       </c>
@@ -5983,7 +5984,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>147</v>
       </c>
@@ -6006,7 +6007,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>148</v>
       </c>
@@ -6029,7 +6030,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>149</v>
       </c>
@@ -6052,7 +6053,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>150</v>
       </c>
@@ -6075,7 +6076,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>151</v>
       </c>
@@ -6098,7 +6099,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>152</v>
       </c>
@@ -6121,7 +6122,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>153</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>154</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>155</v>
       </c>
@@ -6190,7 +6191,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>156</v>
       </c>
@@ -6213,7 +6214,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>157</v>
       </c>
@@ -6236,7 +6237,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>158</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>159</v>
       </c>
@@ -6282,7 +6283,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>160</v>
       </c>
@@ -6305,7 +6306,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>161</v>
       </c>
@@ -6328,7 +6329,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>162</v>
       </c>
@@ -6351,7 +6352,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>163</v>
       </c>
@@ -6374,7 +6375,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>164</v>
       </c>
@@ -6397,7 +6398,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>165</v>
       </c>
@@ -6420,7 +6421,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>166</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>167</v>
       </c>
@@ -6466,7 +6467,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>168</v>
       </c>
@@ -6489,7 +6490,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>169</v>
       </c>
@@ -6512,7 +6513,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>170</v>
       </c>
@@ -6535,7 +6536,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>171</v>
       </c>
@@ -6558,7 +6559,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>172</v>
       </c>
@@ -6581,7 +6582,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>173</v>
       </c>
@@ -6604,7 +6605,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>174</v>
       </c>
@@ -6627,7 +6628,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>175</v>
       </c>
@@ -6650,7 +6651,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>176</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>177</v>
       </c>
@@ -6696,7 +6697,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>239</v>
       </c>
@@ -6719,7 +6720,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>178</v>
       </c>
@@ -6742,7 +6743,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>179</v>
       </c>
@@ -6765,7 +6766,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>180</v>
       </c>
@@ -6788,7 +6789,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>181</v>
       </c>
@@ -6811,7 +6812,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>182</v>
       </c>
@@ -6834,7 +6835,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>183</v>
       </c>
@@ -6857,7 +6858,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>184</v>
       </c>
@@ -6880,7 +6881,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>186</v>
       </c>
@@ -6903,7 +6904,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>187</v>
       </c>
@@ -6926,7 +6927,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>188</v>
       </c>
@@ -6949,7 +6950,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>189</v>
       </c>
@@ -6972,7 +6973,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>190</v>
       </c>
@@ -6995,7 +6996,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>191</v>
       </c>
@@ -7018,7 +7019,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>192</v>
       </c>
@@ -7041,7 +7042,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>193</v>
       </c>
@@ -7064,7 +7065,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>194</v>
       </c>
@@ -7087,7 +7088,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>195</v>
       </c>
@@ -7110,7 +7111,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>196</v>
       </c>
@@ -7133,7 +7134,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>197</v>
       </c>
@@ -7156,7 +7157,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>199</v>
       </c>
@@ -7179,7 +7180,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>200</v>
       </c>
@@ -7202,7 +7203,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>201</v>
       </c>
@@ -7225,7 +7226,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>202</v>
       </c>
@@ -7248,7 +7249,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>203</v>
       </c>
@@ -7271,7 +7272,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>204</v>
       </c>
@@ -7294,7 +7295,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>205</v>
       </c>
@@ -7317,7 +7318,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>206</v>
       </c>
@@ -7340,7 +7341,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>207</v>
       </c>
@@ -7363,7 +7364,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>208</v>
       </c>
@@ -7386,7 +7387,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>209</v>
       </c>
@@ -7409,7 +7410,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>210</v>
       </c>
@@ -7432,7 +7433,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>211</v>
       </c>
@@ -7455,7 +7456,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>212</v>
       </c>
@@ -7478,7 +7479,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>213</v>
       </c>
@@ -7501,7 +7502,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>214</v>
       </c>
@@ -7524,7 +7525,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>215</v>
       </c>
@@ -7547,7 +7548,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>216</v>
       </c>
@@ -7570,7 +7571,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>217</v>
       </c>
@@ -7593,7 +7594,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>218</v>
       </c>
@@ -7616,7 +7617,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>219</v>
       </c>
@@ -7639,7 +7640,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>220</v>
       </c>
@@ -7662,7 +7663,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>221</v>
       </c>
@@ -7685,7 +7686,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>222</v>
       </c>
@@ -7708,7 +7709,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>223</v>
       </c>
@@ -7731,7 +7732,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>224</v>
       </c>
@@ -7754,7 +7755,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>225</v>
       </c>
@@ -7777,7 +7778,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>226</v>
       </c>
@@ -7800,7 +7801,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>227</v>
       </c>
@@ -7823,7 +7824,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>228</v>
       </c>
@@ -7846,7 +7847,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>229</v>
       </c>
@@ -7869,7 +7870,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>230</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>231</v>
       </c>
@@ -7915,7 +7916,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>232</v>
       </c>
@@ -7938,7 +7939,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>233</v>
       </c>
@@ -7961,7 +7962,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>234</v>
       </c>
@@ -7984,7 +7985,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>235</v>
       </c>
@@ -8007,7 +8008,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>236</v>
       </c>
@@ -8030,7 +8031,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>237</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>238</v>
       </c>
@@ -8076,7 +8077,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>94</v>
       </c>
@@ -8108,20 +8109,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
reserviert Thangka 35 Buddhas gold
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9C1B64BC-DDE5-45F3-AC78-6B4AF04A251C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BAEA79EA-FE27-4834-B0EA-EAD709D05AB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2076" yWindow="684" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2684,8 +2684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6608,8 +6608,8 @@
       <c r="D171" s="1">
         <v>499</v>
       </c>
-      <c r="E171">
-        <v>1</v>
+      <c r="E171" s="2">
+        <v>0</v>
       </c>
       <c r="F171" t="s">
         <v>503</v>

</xml_diff>

<commit_message>
Included CategoryFriendlyName in Excel Sheet for Räuchergefäße
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Documents\code\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E8267210-1CA4-4BBC-AD78-5ECBBDE01FC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690FE0BB-CA41-4F05-BF4D-BDE00AD9DAB8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2076" yWindow="684" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="690" windowWidth="23040" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="595">
   <si>
     <t>Name</t>
   </si>
@@ -1618,9 +1618,6 @@
     <t>WBWT028.JPG, WBWT029.JPG</t>
   </si>
   <si>
-    <t>WBWT012.JPG, WBWT011.JPG, WBWT014.JPG, WBWT013.JPG, WBWT016.JPG, WBWT017.JPG, WBWT015.JPG,</t>
-  </si>
-  <si>
     <t>WG001.JPG</t>
   </si>
   <si>
@@ -1812,6 +1809,15 @@
   </si>
   <si>
     <t xml:space="preserve">Stupa Stein 27cm </t>
+  </si>
+  <si>
+    <t>WBWT012.JPG, WBWT011.JPG, WBWT014.JPG, WBWT013.JPG, WBWT016.JPG, WBWT017.JPG, WBWT015.JPG</t>
+  </si>
+  <si>
+    <t>FriendlyCategoryName</t>
+  </si>
+  <si>
+    <t>weiteres - Raeucherzubehoer</t>
   </si>
 </sst>
 </file>
@@ -2684,18 +2690,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A209" sqref="A209:XFD209"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" customWidth="1"/>
-    <col min="6" max="6" width="65.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>354</v>
       </c>
@@ -2717,8 +2724,11 @@
       <c r="G1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2741,7 +2751,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2764,7 +2774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2787,7 +2797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2810,7 +2820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2833,7 +2843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2856,7 +2866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2879,7 +2889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2902,7 +2912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2925,7 +2935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2948,7 +2958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2971,7 +2981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2994,7 +3004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3017,7 +3027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3040,7 +3050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3063,7 +3073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3086,7 +3096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3109,7 +3119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3132,7 +3142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3155,7 +3165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3178,7 +3188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -3201,7 +3211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -3224,7 +3234,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -3247,7 +3257,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -3270,7 +3280,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -3293,7 +3303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -3316,7 +3326,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -3339,7 +3349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -3362,7 +3372,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -3385,7 +3395,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -3408,7 +3418,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -3431,7 +3441,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -3454,7 +3464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -3477,7 +3487,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
@@ -3500,7 +3510,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -3523,7 +3533,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
@@ -3546,7 +3556,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -3592,7 +3602,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3615,7 +3625,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
@@ -3638,7 +3648,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
@@ -3661,7 +3671,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
@@ -3684,7 +3694,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
@@ -3707,7 +3717,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
@@ -3730,7 +3740,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
@@ -3753,7 +3763,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>49</v>
       </c>
@@ -3776,7 +3786,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>241</v>
       </c>
@@ -3784,7 +3794,7 @@
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D48" s="1">
         <v>250</v>
@@ -3793,13 +3803,13 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
+        <v>586</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>587</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>50</v>
       </c>
@@ -3822,7 +3832,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>51</v>
       </c>
@@ -3845,7 +3855,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>52</v>
       </c>
@@ -3868,7 +3878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>53</v>
       </c>
@@ -3891,7 +3901,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>54</v>
       </c>
@@ -3914,7 +3924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>56</v>
       </c>
@@ -3937,7 +3947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>57</v>
       </c>
@@ -3960,7 +3970,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>58</v>
       </c>
@@ -3983,7 +3993,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>59</v>
       </c>
@@ -4006,7 +4016,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>60</v>
       </c>
@@ -4029,7 +4039,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>61</v>
       </c>
@@ -4037,7 +4047,7 @@
         <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D59" s="1">
         <v>499</v>
@@ -4052,7 +4062,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>63</v>
       </c>
@@ -4075,7 +4085,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>240</v>
       </c>
@@ -4083,7 +4093,7 @@
         <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D61" s="1">
         <v>1000</v>
@@ -4092,13 +4102,13 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>66</v>
       </c>
@@ -4121,7 +4131,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>67</v>
       </c>
@@ -4144,7 +4154,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>68</v>
       </c>
@@ -4167,7 +4177,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>69</v>
       </c>
@@ -4190,7 +4200,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>70</v>
       </c>
@@ -4207,13 +4217,13 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G66" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>71</v>
       </c>
@@ -4230,13 +4240,13 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G67" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>72</v>
       </c>
@@ -4253,13 +4263,13 @@
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G68" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>73</v>
       </c>
@@ -4276,13 +4286,13 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G69" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>74</v>
       </c>
@@ -4299,13 +4309,13 @@
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G70" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>75</v>
       </c>
@@ -4322,13 +4332,13 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G71" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>76</v>
       </c>
@@ -4345,13 +4355,13 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G72" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>77</v>
       </c>
@@ -4368,13 +4378,13 @@
         <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G73" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>78</v>
       </c>
@@ -4391,13 +4401,13 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G74" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>79</v>
       </c>
@@ -4414,13 +4424,13 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G75" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>80</v>
       </c>
@@ -4437,18 +4447,18 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C77" t="s">
         <v>121</v>
@@ -4466,12 +4476,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C78" t="s">
         <v>129</v>
@@ -4489,12 +4499,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C79" t="s">
         <v>128</v>
@@ -4512,12 +4522,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C80" t="s">
         <v>125</v>
@@ -4535,12 +4545,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C81" t="s">
         <v>123</v>
@@ -4558,12 +4568,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C82" t="s">
         <v>124</v>
@@ -4581,12 +4591,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C83" t="s">
         <v>118</v>
@@ -4604,12 +4614,12 @@
         <v>340</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C84" t="s">
         <v>131</v>
@@ -4627,12 +4637,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C85" t="s">
         <v>118</v>
@@ -4650,12 +4660,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>91</v>
       </c>
       <c r="B86" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C86" t="s">
         <v>341</v>
@@ -4673,12 +4683,12 @@
         <v>341</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C87" t="s">
         <v>120</v>
@@ -4696,12 +4706,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>95</v>
       </c>
       <c r="B88" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C88" t="s">
         <v>135</v>
@@ -4719,12 +4729,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>96</v>
       </c>
       <c r="B89" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C89" t="s">
         <v>342</v>
@@ -4742,12 +4752,12 @@
         <v>342</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C90" t="s">
         <v>134</v>
@@ -4765,12 +4775,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>98</v>
       </c>
       <c r="B91" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C91" t="s">
         <v>136</v>
@@ -4788,12 +4798,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C92" t="s">
         <v>343</v>
@@ -4811,12 +4821,12 @@
         <v>343</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>100</v>
       </c>
       <c r="B93" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C93" t="s">
         <v>133</v>
@@ -4834,12 +4844,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>101</v>
       </c>
       <c r="B94" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C94" t="s">
         <v>344</v>
@@ -4857,12 +4867,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>103</v>
       </c>
       <c r="B95" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>137</v>
@@ -4884,12 +4894,12 @@
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C96" t="s">
         <v>139</v>
@@ -4907,7 +4917,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>105</v>
       </c>
@@ -4930,7 +4940,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>106</v>
       </c>
@@ -4953,7 +4963,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>107</v>
       </c>
@@ -4976,7 +4986,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>108</v>
       </c>
@@ -4999,7 +5009,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>109</v>
       </c>
@@ -5022,7 +5032,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>110</v>
       </c>
@@ -5045,7 +5055,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>111</v>
       </c>
@@ -5068,7 +5078,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>112</v>
       </c>
@@ -5091,7 +5101,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>113</v>
       </c>
@@ -5114,7 +5124,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>114</v>
       </c>
@@ -5137,7 +5147,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>115</v>
       </c>
@@ -5160,7 +5170,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>116</v>
       </c>
@@ -5183,7 +5193,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>117</v>
       </c>
@@ -5206,7 +5216,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>118</v>
       </c>
@@ -5229,7 +5239,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>119</v>
       </c>
@@ -5252,7 +5262,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>120</v>
       </c>
@@ -5275,7 +5285,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>121</v>
       </c>
@@ -5298,7 +5308,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>122</v>
       </c>
@@ -5321,7 +5331,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>123</v>
       </c>
@@ -5344,7 +5354,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>124</v>
       </c>
@@ -5367,7 +5377,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>125</v>
       </c>
@@ -5390,7 +5400,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>126</v>
       </c>
@@ -5413,7 +5423,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>127</v>
       </c>
@@ -5436,7 +5446,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>128</v>
       </c>
@@ -5459,7 +5469,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>129</v>
       </c>
@@ -5482,7 +5492,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>130</v>
       </c>
@@ -5505,7 +5515,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>131</v>
       </c>
@@ -5528,7 +5538,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>132</v>
       </c>
@@ -5551,7 +5561,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>133</v>
       </c>
@@ -5574,7 +5584,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>134</v>
       </c>
@@ -5597,7 +5607,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>135</v>
       </c>
@@ -5620,7 +5630,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>136</v>
       </c>
@@ -5643,7 +5653,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>137</v>
       </c>
@@ -5666,7 +5676,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>138</v>
       </c>
@@ -5689,7 +5699,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>139</v>
       </c>
@@ -5712,7 +5722,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>140</v>
       </c>
@@ -5735,7 +5745,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>141</v>
       </c>
@@ -5758,7 +5768,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>142</v>
       </c>
@@ -5781,7 +5791,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>143</v>
       </c>
@@ -5804,7 +5814,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>144</v>
       </c>
@@ -5827,7 +5837,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>145</v>
       </c>
@@ -5850,12 +5860,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>146</v>
       </c>
       <c r="B138" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C138" t="s">
         <v>201</v>
@@ -5867,18 +5877,18 @@
         <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G138" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>147</v>
       </c>
       <c r="B139" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C139" t="s">
         <v>202</v>
@@ -5890,18 +5900,18 @@
         <v>1</v>
       </c>
       <c r="F139" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G139" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>148</v>
       </c>
       <c r="B140" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C140" t="s">
         <v>203</v>
@@ -5913,18 +5923,18 @@
         <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G140" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>149</v>
       </c>
       <c r="B141" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C141" t="s">
         <v>195</v>
@@ -5936,18 +5946,18 @@
         <v>1</v>
       </c>
       <c r="F141" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G141" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>150</v>
       </c>
       <c r="B142" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C142" t="s">
         <v>196</v>
@@ -5959,18 +5969,18 @@
         <v>1</v>
       </c>
       <c r="F142" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G142" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>151</v>
       </c>
       <c r="B143" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C143" t="s">
         <v>197</v>
@@ -5982,18 +5992,18 @@
         <v>1</v>
       </c>
       <c r="F143" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G143" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>152</v>
       </c>
       <c r="B144" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C144" t="s">
         <v>199</v>
@@ -6005,18 +6015,18 @@
         <v>1</v>
       </c>
       <c r="F144" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G144" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>153</v>
       </c>
       <c r="B145" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C145" t="s">
         <v>193</v>
@@ -6028,13 +6038,13 @@
         <v>1</v>
       </c>
       <c r="F145" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G145" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>154</v>
       </c>
@@ -6057,7 +6067,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>155</v>
       </c>
@@ -6080,7 +6090,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>156</v>
       </c>
@@ -6103,7 +6113,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>157</v>
       </c>
@@ -6126,7 +6136,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>158</v>
       </c>
@@ -6149,7 +6159,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>159</v>
       </c>
@@ -6172,7 +6182,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>160</v>
       </c>
@@ -6195,7 +6205,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>161</v>
       </c>
@@ -6218,7 +6228,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>162</v>
       </c>
@@ -6241,7 +6251,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>163</v>
       </c>
@@ -6264,7 +6274,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>164</v>
       </c>
@@ -6287,7 +6297,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>165</v>
       </c>
@@ -6310,7 +6320,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>166</v>
       </c>
@@ -6333,7 +6343,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>167</v>
       </c>
@@ -6356,7 +6366,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>168</v>
       </c>
@@ -6379,7 +6389,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>169</v>
       </c>
@@ -6402,7 +6412,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>170</v>
       </c>
@@ -6425,7 +6435,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>171</v>
       </c>
@@ -6448,7 +6458,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>172</v>
       </c>
@@ -6471,7 +6481,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>173</v>
       </c>
@@ -6494,7 +6504,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>175</v>
       </c>
@@ -6517,7 +6527,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>176</v>
       </c>
@@ -6540,7 +6550,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>239</v>
       </c>
@@ -6548,7 +6558,7 @@
         <v>237</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D168" s="4">
         <v>400</v>
@@ -6557,13 +6567,13 @@
         <v>1</v>
       </c>
       <c r="F168" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="G168" t="s">
         <v>584</v>
       </c>
-      <c r="G168" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>178</v>
       </c>
@@ -6586,12 +6596,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>179</v>
       </c>
       <c r="B170" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C170" t="s">
         <v>346</v>
@@ -6609,12 +6619,12 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>180</v>
       </c>
       <c r="B171" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C171" t="s">
         <v>257</v>
@@ -6632,12 +6642,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>181</v>
       </c>
       <c r="B172" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C172" t="s">
         <v>252</v>
@@ -6655,12 +6665,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>182</v>
       </c>
       <c r="B173" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C173" t="s">
         <v>261</v>
@@ -6678,12 +6688,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>183</v>
       </c>
       <c r="B174" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C174" t="s">
         <v>250</v>
@@ -6701,12 +6711,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>184</v>
       </c>
       <c r="B175" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C175" t="s">
         <v>260</v>
@@ -6724,12 +6734,12 @@
         <v>260</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>186</v>
       </c>
       <c r="B176" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C176" t="s">
         <v>259</v>
@@ -6747,12 +6757,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>187</v>
       </c>
       <c r="B177" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C177" t="s">
         <v>251</v>
@@ -6770,12 +6780,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>188</v>
       </c>
       <c r="B178" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C178" t="s">
         <v>255</v>
@@ -6793,12 +6803,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>189</v>
       </c>
       <c r="B179" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C179" t="s">
         <v>254</v>
@@ -6816,12 +6826,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>190</v>
       </c>
       <c r="B180" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C180" t="s">
         <v>249</v>
@@ -6839,12 +6849,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>191</v>
       </c>
       <c r="B181" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C181" t="s">
         <v>256</v>
@@ -6862,12 +6872,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>192</v>
       </c>
       <c r="B182" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C182" t="s">
         <v>268</v>
@@ -6885,12 +6895,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>193</v>
       </c>
       <c r="B183" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C183" t="s">
         <v>266</v>
@@ -6908,12 +6918,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>194</v>
       </c>
       <c r="B184" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C184" t="s">
         <v>267</v>
@@ -6931,12 +6941,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>195</v>
       </c>
       <c r="B185" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C185" t="s">
         <v>265</v>
@@ -6954,12 +6964,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>196</v>
       </c>
       <c r="B186" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C186" t="s">
         <v>270</v>
@@ -6977,12 +6987,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>197</v>
       </c>
       <c r="B187" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C187" t="s">
         <v>271</v>
@@ -7000,12 +7010,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>199</v>
       </c>
       <c r="B188" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C188" t="s">
         <v>263</v>
@@ -7023,12 +7033,12 @@
         <v>262</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>200</v>
       </c>
       <c r="B189" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C189" t="s">
         <v>269</v>
@@ -7046,12 +7056,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>201</v>
       </c>
       <c r="B190" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C190" t="s">
         <v>273</v>
@@ -7069,12 +7079,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>202</v>
       </c>
       <c r="B191" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C191" t="s">
         <v>275</v>
@@ -7086,13 +7096,13 @@
         <v>1</v>
       </c>
       <c r="F191" t="s">
-        <v>528</v>
+        <v>592</v>
       </c>
       <c r="G191" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>203</v>
       </c>
@@ -7109,13 +7119,13 @@
         <v>1</v>
       </c>
       <c r="F192" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G192" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>204</v>
       </c>
@@ -7132,13 +7142,13 @@
         <v>1</v>
       </c>
       <c r="F193" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G193" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>205</v>
       </c>
@@ -7155,13 +7165,13 @@
         <v>1</v>
       </c>
       <c r="F194" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G194" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>206</v>
       </c>
@@ -7178,13 +7188,13 @@
         <v>1</v>
       </c>
       <c r="F195" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G195" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>207</v>
       </c>
@@ -7201,13 +7211,13 @@
         <v>1</v>
       </c>
       <c r="F196" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G196" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>208</v>
       </c>
@@ -7224,13 +7234,13 @@
         <v>1</v>
       </c>
       <c r="F197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G197" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>209</v>
       </c>
@@ -7247,13 +7257,13 @@
         <v>1</v>
       </c>
       <c r="F198" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G198" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>210</v>
       </c>
@@ -7270,13 +7280,13 @@
         <v>1</v>
       </c>
       <c r="F199" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G199" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>211</v>
       </c>
@@ -7293,13 +7303,13 @@
         <v>1</v>
       </c>
       <c r="F200" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G200" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>212</v>
       </c>
@@ -7316,18 +7326,18 @@
         <v>1</v>
       </c>
       <c r="F201" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G201" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>213</v>
       </c>
       <c r="B202" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C202" t="s">
         <v>299</v>
@@ -7339,18 +7349,21 @@
         <v>1</v>
       </c>
       <c r="F202" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G202" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H202" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>214</v>
       </c>
       <c r="B203" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C203" t="s">
         <v>298</v>
@@ -7362,18 +7375,21 @@
         <v>1</v>
       </c>
       <c r="F203" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G203" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H203" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>215</v>
       </c>
       <c r="B204" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C204" t="s">
         <v>300</v>
@@ -7385,18 +7401,21 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G204" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H204" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>216</v>
       </c>
       <c r="B205" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C205" t="s">
         <v>297</v>
@@ -7408,13 +7427,16 @@
         <v>1</v>
       </c>
       <c r="F205" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G205" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H205" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>217</v>
       </c>
@@ -7431,13 +7453,13 @@
         <v>1</v>
       </c>
       <c r="F206" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G206" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>218</v>
       </c>
@@ -7454,13 +7476,13 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G207" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>219</v>
       </c>
@@ -7477,13 +7499,13 @@
         <v>1</v>
       </c>
       <c r="F208" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G208" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>221</v>
       </c>
@@ -7500,13 +7522,13 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G209" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>222</v>
       </c>
@@ -7523,13 +7545,13 @@
         <v>1</v>
       </c>
       <c r="F210" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G210" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>223</v>
       </c>
@@ -7546,13 +7568,13 @@
         <v>1</v>
       </c>
       <c r="F211" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G211" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>224</v>
       </c>
@@ -7569,13 +7591,13 @@
         <v>1</v>
       </c>
       <c r="F212" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G212" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>225</v>
       </c>
@@ -7592,13 +7614,13 @@
         <v>1</v>
       </c>
       <c r="F213" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G213" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>226</v>
       </c>
@@ -7615,13 +7637,13 @@
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G214" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>227</v>
       </c>
@@ -7638,13 +7660,13 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G215" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>228</v>
       </c>
@@ -7661,13 +7683,13 @@
         <v>1</v>
       </c>
       <c r="F216" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G216" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>229</v>
       </c>
@@ -7684,13 +7706,13 @@
         <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G217" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>230</v>
       </c>
@@ -7707,13 +7729,13 @@
         <v>1</v>
       </c>
       <c r="F218" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G218" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>231</v>
       </c>
@@ -7730,13 +7752,13 @@
         <v>1</v>
       </c>
       <c r="F219" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G219" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>232</v>
       </c>
@@ -7753,13 +7775,13 @@
         <v>1</v>
       </c>
       <c r="F220" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G220" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>233</v>
       </c>
@@ -7776,13 +7798,13 @@
         <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G221" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>234</v>
       </c>
@@ -7799,13 +7821,13 @@
         <v>1</v>
       </c>
       <c r="F222" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G222" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>235</v>
       </c>
@@ -7822,13 +7844,13 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G223" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>236</v>
       </c>
@@ -7845,13 +7867,13 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G224" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>237</v>
       </c>
@@ -7868,13 +7890,13 @@
         <v>1</v>
       </c>
       <c r="F225" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G225" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>238</v>
       </c>
@@ -7891,18 +7913,18 @@
         <v>1</v>
       </c>
       <c r="F226" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G226" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>94</v>
       </c>
       <c r="B227" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C227" t="s">
         <v>127</v>
@@ -7914,13 +7936,13 @@
         <v>1</v>
       </c>
       <c r="F227" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G227" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D229" s="1"/>
     </row>
   </sheetData>
@@ -7940,13 +7962,13 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>177</v>
       </c>
@@ -7954,7 +7976,7 @@
         <v>237</v>
       </c>
       <c r="C1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D1" s="1">
         <v>999</v>
@@ -7969,7 +7991,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>177</v>
       </c>
@@ -7977,7 +7999,7 @@
         <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D2" s="1">
         <v>999</v>
@@ -7992,7 +8014,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>174</v>
       </c>
@@ -8015,7 +8037,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>62</v>
       </c>
@@ -8038,7 +8060,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>48</v>
       </c>
@@ -8061,7 +8083,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>55</v>
       </c>
@@ -8084,7 +8106,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>64</v>
       </c>
@@ -8107,7 +8129,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>220</v>
       </c>
@@ -8124,7 +8146,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G8" t="s">
         <v>305</v>

</xml_diff>

<commit_message>
auf der zweiten Seite mit 0 gewechselt
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8D4C85-87BB-4403-B269-FBAE5646EAA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770170FB-5DBB-402A-8DF8-371AB539402B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2076" yWindow="696" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2076" yWindow="696" windowWidth="23040" windowHeight="9636" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="671">
   <si>
     <t>Name</t>
   </si>
@@ -1793,10 +1793,6 @@
   </si>
   <si>
     <t>BRat003.JPG</t>
-  </si>
-  <si>
-    <t>Der Silberanteil ist 90%.
- Das Gewicht der Statue ist 80 Gramm, das bedeutet der Wert des Materials beträgt schon ca. 90 Euro( Preisbasis 100 g. Silber 120 Euro).Außerdem sollte berücksichtigt werden, dass die Verarbeitung von einer Silberstatue viel aufwendiger ist.</t>
   </si>
   <si>
     <t>Die Fünf Buddhas ( Jinas ) in Silber</t>
@@ -2939,7 +2935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A240" sqref="A240:XFD240"/>
     </sheetView>
   </sheetViews>
@@ -2975,7 +2971,7 @@
         <v>359</v>
       </c>
       <c r="H1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -4272,7 +4268,7 @@
         <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D58" s="1">
         <v>499</v>
@@ -7511,7 +7507,7 @@
         <v>299</v>
       </c>
       <c r="H198" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
@@ -7537,7 +7533,7 @@
         <v>298</v>
       </c>
       <c r="H199" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
@@ -7563,7 +7559,7 @@
         <v>300</v>
       </c>
       <c r="H200" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
@@ -7589,7 +7585,7 @@
         <v>297</v>
       </c>
       <c r="H201" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
@@ -8080,10 +8076,10 @@
         <v>251</v>
       </c>
       <c r="B223" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C223" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D223" s="1">
         <v>14800</v>
@@ -8092,13 +8088,13 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
+        <v>599</v>
+      </c>
+      <c r="G223" t="s">
         <v>600</v>
       </c>
-      <c r="G223" t="s">
-        <v>601</v>
-      </c>
       <c r="H223" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
@@ -8106,10 +8102,10 @@
         <v>252</v>
       </c>
       <c r="B224" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C224" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D224" s="1">
         <v>580</v>
@@ -8118,13 +8114,13 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
+        <v>602</v>
+      </c>
+      <c r="G224" t="s">
         <v>603</v>
       </c>
-      <c r="G224" t="s">
-        <v>604</v>
-      </c>
       <c r="H224" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
@@ -8132,10 +8128,10 @@
         <v>253</v>
       </c>
       <c r="B225" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C225" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D225" s="1">
         <v>3800</v>
@@ -8144,13 +8140,13 @@
         <v>1</v>
       </c>
       <c r="F225" t="s">
+        <v>605</v>
+      </c>
+      <c r="G225" t="s">
         <v>606</v>
       </c>
-      <c r="G225" t="s">
-        <v>607</v>
-      </c>
       <c r="H225" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
@@ -8158,10 +8154,10 @@
         <v>255</v>
       </c>
       <c r="B226" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C226" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D226" s="1">
         <v>6800</v>
@@ -8170,13 +8166,13 @@
         <v>1</v>
       </c>
       <c r="F226" t="s">
+        <v>611</v>
+      </c>
+      <c r="G226" t="s">
         <v>612</v>
       </c>
-      <c r="G226" t="s">
-        <v>613</v>
-      </c>
       <c r="H226" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
@@ -8184,10 +8180,10 @@
         <v>256</v>
       </c>
       <c r="B227" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C227" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D227" s="1">
         <v>599</v>
@@ -8196,13 +8192,13 @@
         <v>1</v>
       </c>
       <c r="F227" t="s">
+        <v>614</v>
+      </c>
+      <c r="G227" t="s">
         <v>615</v>
       </c>
-      <c r="G227" t="s">
-        <v>616</v>
-      </c>
       <c r="H227" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
@@ -8210,10 +8206,10 @@
         <v>257</v>
       </c>
       <c r="B228" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C228" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D228" s="1">
         <v>799</v>
@@ -8222,13 +8218,13 @@
         <v>1</v>
       </c>
       <c r="F228" t="s">
+        <v>617</v>
+      </c>
+      <c r="G228" t="s">
         <v>618</v>
       </c>
-      <c r="G228" t="s">
-        <v>619</v>
-      </c>
       <c r="H228" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
@@ -8236,10 +8232,10 @@
         <v>258</v>
       </c>
       <c r="B229" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C229" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D229" s="1">
         <v>1700</v>
@@ -8248,13 +8244,13 @@
         <v>1</v>
       </c>
       <c r="F229" t="s">
+        <v>620</v>
+      </c>
+      <c r="G229" t="s">
         <v>621</v>
       </c>
-      <c r="G229" t="s">
-        <v>622</v>
-      </c>
       <c r="H229" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
@@ -8262,10 +8258,10 @@
         <v>260</v>
       </c>
       <c r="B230" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C230" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D230" s="1">
         <v>1990</v>
@@ -8274,13 +8270,13 @@
         <v>1</v>
       </c>
       <c r="F230" t="s">
+        <v>626</v>
+      </c>
+      <c r="G230" t="s">
         <v>627</v>
       </c>
-      <c r="G230" t="s">
-        <v>628</v>
-      </c>
       <c r="H230" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
@@ -8288,10 +8284,10 @@
         <v>261</v>
       </c>
       <c r="B231" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C231" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D231" s="1">
         <v>2999</v>
@@ -8300,13 +8296,13 @@
         <v>1</v>
       </c>
       <c r="F231" t="s">
+        <v>629</v>
+      </c>
+      <c r="G231" t="s">
         <v>630</v>
       </c>
-      <c r="G231" t="s">
-        <v>631</v>
-      </c>
       <c r="H231" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
@@ -8314,10 +8310,10 @@
         <v>262</v>
       </c>
       <c r="B232" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C232" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D232" s="1">
         <v>1400</v>
@@ -8326,10 +8322,10 @@
         <v>1</v>
       </c>
       <c r="F232" t="s">
+        <v>632</v>
+      </c>
+      <c r="G232" t="s">
         <v>633</v>
-      </c>
-      <c r="G232" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
@@ -8337,10 +8333,10 @@
         <v>263</v>
       </c>
       <c r="B233" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C233" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D233" s="1">
         <v>999</v>
@@ -8349,10 +8345,10 @@
         <v>1</v>
       </c>
       <c r="F233" t="s">
+        <v>635</v>
+      </c>
+      <c r="G233" t="s">
         <v>636</v>
-      </c>
-      <c r="G233" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
@@ -8360,10 +8356,10 @@
         <v>264</v>
       </c>
       <c r="B234" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C234" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D234" s="1">
         <v>1500</v>
@@ -8372,10 +8368,10 @@
         <v>1</v>
       </c>
       <c r="F234" t="s">
+        <v>638</v>
+      </c>
+      <c r="G234" t="s">
         <v>639</v>
-      </c>
-      <c r="G234" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
@@ -8383,10 +8379,10 @@
         <v>265</v>
       </c>
       <c r="B235" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C235" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D235" s="1">
         <v>1299</v>
@@ -8395,10 +8391,10 @@
         <v>0</v>
       </c>
       <c r="F235" t="s">
+        <v>641</v>
+      </c>
+      <c r="G235" t="s">
         <v>642</v>
-      </c>
-      <c r="G235" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
@@ -8406,10 +8402,10 @@
         <v>266</v>
       </c>
       <c r="B236" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C236" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D236" s="1">
         <v>799</v>
@@ -8418,10 +8414,10 @@
         <v>1</v>
       </c>
       <c r="F236" t="s">
+        <v>644</v>
+      </c>
+      <c r="G236" t="s">
         <v>645</v>
-      </c>
-      <c r="G236" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
@@ -8432,7 +8428,7 @@
         <v>27</v>
       </c>
       <c r="C237" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D237" s="1">
         <v>849</v>
@@ -8441,10 +8437,10 @@
         <v>1</v>
       </c>
       <c r="F237" t="s">
+        <v>647</v>
+      </c>
+      <c r="G237" t="s">
         <v>648</v>
-      </c>
-      <c r="G237" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
@@ -8455,7 +8451,7 @@
         <v>37</v>
       </c>
       <c r="C238" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D238" s="1">
         <v>450</v>
@@ -8464,10 +8460,10 @@
         <v>1</v>
       </c>
       <c r="F238" t="s">
+        <v>650</v>
+      </c>
+      <c r="G238" t="s">
         <v>651</v>
-      </c>
-      <c r="G238" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
@@ -8478,7 +8474,7 @@
         <v>580</v>
       </c>
       <c r="C239" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D239" s="1">
         <v>699</v>
@@ -8487,10 +8483,10 @@
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G239" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
@@ -8501,7 +8497,7 @@
         <v>580</v>
       </c>
       <c r="C240" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D240" s="1">
         <v>999</v>
@@ -8510,10 +8506,10 @@
         <v>1</v>
       </c>
       <c r="F240" t="s">
+        <v>658</v>
+      </c>
+      <c r="G240" t="s">
         <v>659</v>
-      </c>
-      <c r="G240" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.3">
@@ -8521,10 +8517,10 @@
         <v>272</v>
       </c>
       <c r="B241" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C241" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D241" s="1">
         <v>599</v>
@@ -8533,13 +8529,13 @@
         <v>1</v>
       </c>
       <c r="F241" t="s">
+        <v>661</v>
+      </c>
+      <c r="G241" t="s">
         <v>662</v>
       </c>
-      <c r="G241" t="s">
-        <v>663</v>
-      </c>
       <c r="H241" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
@@ -8550,7 +8546,7 @@
         <v>62</v>
       </c>
       <c r="C242" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D242" s="1">
         <v>1100</v>
@@ -8559,10 +8555,10 @@
         <v>1</v>
       </c>
       <c r="F242" t="s">
+        <v>664</v>
+      </c>
+      <c r="G242" t="s">
         <v>665</v>
-      </c>
-      <c r="G242" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -8573,7 +8569,7 @@
         <v>581</v>
       </c>
       <c r="C243" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D243" s="1">
         <v>1999</v>
@@ -8582,10 +8578,10 @@
         <v>1</v>
       </c>
       <c r="F243" t="s">
+        <v>667</v>
+      </c>
+      <c r="G243" t="s">
         <v>668</v>
-      </c>
-      <c r="G243" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
@@ -8602,10 +8598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8622,7 +8618,7 @@
         <v>237</v>
       </c>
       <c r="C1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D1" s="1">
         <v>999</v>
@@ -8645,7 +8641,7 @@
         <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D2" s="1">
         <v>999</v>
@@ -8803,25 +8799,25 @@
         <v>259</v>
       </c>
       <c r="B9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D9" s="1">
         <v>9800</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
+        <v>623</v>
+      </c>
+      <c r="G9" t="s">
         <v>624</v>
       </c>
-      <c r="G9" t="s">
-        <v>625</v>
-      </c>
       <c r="H9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -8838,7 +8834,7 @@
         <v>1299</v>
       </c>
       <c r="E10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>569</v>
@@ -8861,10 +8857,10 @@
         <v>1299</v>
       </c>
       <c r="E11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G11" t="s">
         <v>274</v>
@@ -8884,7 +8880,7 @@
         <v>1299</v>
       </c>
       <c r="E12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>516</v>
@@ -8907,7 +8903,7 @@
         <v>59.9</v>
       </c>
       <c r="E13" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>397</v>
@@ -8921,25 +8917,25 @@
         <v>250</v>
       </c>
       <c r="B14" t="s">
+        <v>594</v>
+      </c>
+      <c r="C14" t="s">
         <v>595</v>
-      </c>
-      <c r="C14" t="s">
-        <v>596</v>
       </c>
       <c r="D14" s="1">
         <v>7800</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
+        <v>596</v>
+      </c>
+      <c r="G14" t="s">
         <v>597</v>
       </c>
-      <c r="G14" t="s">
-        <v>598</v>
-      </c>
       <c r="H14" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -8947,25 +8943,25 @@
         <v>254</v>
       </c>
       <c r="B15" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C15" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D15" s="1">
         <v>29800</v>
       </c>
       <c r="E15" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
+        <v>608</v>
+      </c>
+      <c r="G15" t="s">
         <v>609</v>
       </c>
-      <c r="G15" t="s">
-        <v>610</v>
-      </c>
       <c r="H15" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -8976,43 +8972,41 @@
         <v>580</v>
       </c>
       <c r="C16" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D16" s="1">
         <v>1090</v>
       </c>
       <c r="E16" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
+        <v>655</v>
+      </c>
+      <c r="G16" t="s">
         <v>656</v>
       </c>
-      <c r="G16" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
-      <c r="A29">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>240</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B17" t="s">
         <v>79</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C17" t="s">
+        <v>587</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
         <v>588</v>
       </c>
-      <c r="D29" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>589</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>587</v>
-      </c>
+      <c r="G17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Eine THangka raus genommen und ein paar preise geändert
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770170FB-5DBB-402A-8DF8-371AB539402B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E26E585-07A0-4D72-8A7F-202FB8993BE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2076" yWindow="696" windowWidth="23040" windowHeight="9636" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2076" yWindow="696" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -2935,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K245"/>
   <sheetViews>
-    <sheetView topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A240" sqref="A240:XFD240"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4122,29 +4122,6 @@
         <v>335</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>54</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="D52" s="4">
-        <v>399</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>56</v>
@@ -6621,7 +6598,7 @@
         <v>239</v>
       </c>
       <c r="D160" s="1">
-        <v>399</v>
+        <v>450</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -6644,7 +6621,7 @@
         <v>240</v>
       </c>
       <c r="D161" s="4">
-        <v>399</v>
+        <v>500</v>
       </c>
       <c r="E161" s="3">
         <v>1</v>
@@ -6667,7 +6644,7 @@
         <v>241</v>
       </c>
       <c r="D162" s="4">
-        <v>399</v>
+        <v>500</v>
       </c>
       <c r="E162" s="3">
         <v>1</v>
@@ -6759,7 +6736,7 @@
         <v>582</v>
       </c>
       <c r="D166" s="4">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E166" s="3">
         <v>1</v>
@@ -6769,29 +6746,6 @@
       </c>
       <c r="G166" t="s">
         <v>584</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A167">
-        <v>178</v>
-      </c>
-      <c r="B167" t="s">
-        <v>237</v>
-      </c>
-      <c r="C167" t="s">
-        <v>244</v>
-      </c>
-      <c r="D167" s="1">
-        <v>999</v>
-      </c>
-      <c r="E167">
-        <v>1</v>
-      </c>
-      <c r="F167" t="s">
-        <v>507</v>
-      </c>
-      <c r="G167" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -8598,10 +8552,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9008,6 +8962,52 @@
       </c>
       <c r="G17" s="6"/>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D18" s="4">
+        <v>399</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>178</v>
+      </c>
+      <c r="B19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" s="1">
+        <v>999</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>507</v>
+      </c>
+      <c r="G19" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add key for category
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasosterle/Documents/code/react-cintamani/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E26E585-07A0-4D72-8A7F-202FB8993BE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A200069C-FAEB-9D4C-A2BF-BDE7D774D26E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2076" yWindow="696" windowWidth="23040" windowHeight="9636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15980" yWindow="3840" windowWidth="29000" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -2580,48 +2580,48 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2637,7 +2637,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2935,20 +2935,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" customWidth="1"/>
     <col min="3" max="3" width="48.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.83203125" customWidth="1"/>
     <col min="7" max="7" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>354</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>42</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>43</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>44</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>45</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>46</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>49</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>241</v>
       </c>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>50</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>51</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>52</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>53</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>56</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>57</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>58</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>59</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>60</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>61</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>63</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>66</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>67</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>68</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>69</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>70</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>71</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>72</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>73</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>74</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>75</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>76</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>77</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>78</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>79</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>80</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>81</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>82</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>83</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>84</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>85</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>86</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>87</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>88</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>89</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>91</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>93</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>95</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>96</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>97</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>98</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>99</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>100</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>101</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>103</v>
       </c>
@@ -5069,7 +5069,7 @@
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>104</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>105</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>106</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>107</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>108</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>109</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>110</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>111</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>112</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>113</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>114</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>115</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>116</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>117</v>
       </c>
@@ -5391,7 +5391,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>118</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>119</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>120</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>121</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>122</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>123</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>124</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>125</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>126</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>127</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>128</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>129</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>130</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>131</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>132</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>133</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>134</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>135</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>136</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>137</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>138</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>139</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>140</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>141</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>142</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>143</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>144</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>145</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>146</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>147</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>148</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>149</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>150</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>151</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>152</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>153</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>154</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>155</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>156</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>157</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>158</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>159</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>160</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>161</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>162</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>163</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>164</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>165</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>166</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>167</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>168</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>169</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>170</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>171</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>172</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>173</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>175</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>176</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>239</v>
       </c>
@@ -6748,7 +6748,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>179</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>180</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>181</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>182</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>183</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>184</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>186</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>187</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>188</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>190</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>191</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>192</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>193</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>194</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>195</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>196</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>197</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>199</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>200</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>201</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>203</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>204</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>205</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>206</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>207</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>208</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>209</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>210</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>211</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>212</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>213</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>214</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>215</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>216</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>217</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>218</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>219</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>221</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>222</v>
       </c>
@@ -7657,7 +7657,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>223</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>224</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>225</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>226</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>227</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>228</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>229</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>230</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>231</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>232</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>233</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>234</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>235</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>236</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>237</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>238</v>
       </c>
@@ -8025,7 +8025,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>251</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>252</v>
       </c>
@@ -8077,7 +8077,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>253</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>255</v>
       </c>
@@ -8129,7 +8129,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>256</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>257</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>258</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>260</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>261</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>262</v>
       </c>
@@ -8282,7 +8282,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>263</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>264</v>
       </c>
@@ -8328,7 +8328,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>265</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>266</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>267</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>268</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>269</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>271</v>
       </c>
@@ -8466,7 +8466,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>272</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>273</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>274</v>
       </c>
@@ -8538,11 +8538,11 @@
         <v>668</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D245" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A202:G204">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A202:G204">
     <sortCondition ref="D202:D204"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8558,13 +8558,13 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>177</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>177</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>174</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>62</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>48</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>55</v>
       </c>
@@ -8702,7 +8702,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>64</v>
       </c>
@@ -8725,7 +8725,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>220</v>
       </c>
@@ -8748,7 +8748,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>259</v>
       </c>
@@ -8774,7 +8774,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>94</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>202</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>189</v>
       </c>
@@ -8843,7 +8843,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>41</v>
       </c>
@@ -8866,7 +8866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>250</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>254</v>
       </c>
@@ -8918,7 +8918,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>270</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>240</v>
       </c>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>54</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>178</v>
       </c>

</xml_diff>

<commit_message>
Preise von Jonas geändert
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9DA326-2C95-40FA-99EE-53DBD4E769FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D400B13E-AEC0-4429-BD66-E232B49C08DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="669">
   <si>
     <t>Name</t>
   </si>
@@ -750,9 +750,6 @@
     <t>Medizin Buddha Mandala</t>
   </si>
   <si>
-    <t>Shakyamuni Mandala</t>
-  </si>
-  <si>
     <t>Größe: Innen: 63x44 Außen: 125x69</t>
   </si>
   <si>
@@ -1535,9 +1532,6 @@
   </si>
   <si>
     <t>TA250006.JPG, TA250005.JPG</t>
-  </si>
-  <si>
-    <t>TA250004.JPG, TA250003.JPG</t>
   </si>
   <si>
     <t>TA250042.JPG, TA250043.JPG, TA250044.JPG, TA250045.JPG</t>
@@ -2933,10 +2927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K244"/>
+  <dimension ref="A1:K243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B166" sqref="B166"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,28 +2944,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" t="s">
         <v>354</v>
-      </c>
-      <c r="B1" t="s">
-        <v>355</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E1" t="s">
         <v>356</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>357</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>358</v>
       </c>
-      <c r="G1" t="s">
-        <v>359</v>
-      </c>
       <c r="H1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2991,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -3014,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -3037,7 +3031,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -3060,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -3083,7 +3077,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
@@ -3106,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -3129,7 +3123,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -3152,7 +3146,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -3175,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -3198,7 +3192,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
@@ -3221,7 +3215,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G12" t="s">
         <v>13</v>
@@ -3244,7 +3238,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -3267,7 +3261,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -3290,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -3313,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
@@ -3336,7 +3330,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -3359,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -3382,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -3405,7 +3399,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
@@ -3428,7 +3422,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G21" t="s">
         <v>31</v>
@@ -3451,7 +3445,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G22" t="s">
         <v>30</v>
@@ -3474,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -3497,7 +3491,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>35</v>
@@ -3520,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
@@ -3543,7 +3537,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G26" t="s">
         <v>29</v>
@@ -3566,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G27" t="s">
         <v>41</v>
@@ -3589,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G28" t="s">
         <v>38</v>
@@ -3612,7 +3606,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G29" t="s">
         <v>40</v>
@@ -3635,7 +3629,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G30" t="s">
         <v>42</v>
@@ -3658,7 +3652,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G31" t="s">
         <v>39</v>
@@ -3681,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G32" t="s">
         <v>45</v>
@@ -3704,7 +3698,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G33" t="s">
         <v>46</v>
@@ -3727,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G34" t="s">
         <v>47</v>
@@ -3750,7 +3744,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G35" t="s">
         <v>44</v>
@@ -3773,7 +3767,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G36" t="s">
         <v>49</v>
@@ -3796,7 +3790,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G37" t="s">
         <v>53</v>
@@ -3819,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G38" t="s">
         <v>49</v>
@@ -3842,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G39" t="s">
         <v>54</v>
@@ -3865,7 +3859,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G40" t="s">
         <v>49</v>
@@ -3888,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G41" t="s">
         <v>58</v>
@@ -3911,7 +3905,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G42" t="s">
         <v>60</v>
@@ -3934,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G43" t="s">
         <v>67</v>
@@ -3957,7 +3951,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G44" t="s">
         <v>65</v>
@@ -3980,7 +3974,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G45" t="s">
         <v>66</v>
@@ -4003,7 +3997,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G46" t="s">
         <v>69</v>
@@ -4017,7 +4011,7 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D47" s="1">
         <v>250</v>
@@ -4026,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G47" s="6"/>
     </row>
@@ -4047,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G48" t="s">
         <v>70</v>
@@ -4070,7 +4064,7 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G49" t="s">
         <v>76</v>
@@ -4093,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G50" t="s">
         <v>72</v>
@@ -4116,10 +4110,10 @@
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -4139,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G53" t="s">
         <v>83</v>
@@ -4162,7 +4156,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G54" t="s">
         <v>82</v>
@@ -4185,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G55" t="s">
         <v>84</v>
@@ -4208,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G56" t="s">
         <v>88</v>
@@ -4231,7 +4225,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G57" t="s">
         <v>86</v>
@@ -4245,7 +4239,7 @@
         <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D58" s="1">
         <v>499</v>
@@ -4254,10 +4248,10 @@
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -4277,7 +4271,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G59" t="s">
         <v>80</v>
@@ -4300,7 +4294,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G60" t="s">
         <v>97</v>
@@ -4323,7 +4317,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G61" t="s">
         <v>93</v>
@@ -4346,7 +4340,7 @@
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G62" t="s">
         <v>94</v>
@@ -4369,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G63" t="s">
         <v>95</v>
@@ -4380,7 +4374,7 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C64" t="s">
         <v>114</v>
@@ -4392,7 +4386,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="G64" t="s">
         <v>113</v>
@@ -4403,7 +4397,7 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C65" t="s">
         <v>116</v>
@@ -4415,7 +4409,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="G65" t="s">
         <v>115</v>
@@ -4426,7 +4420,7 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C66" t="s">
         <v>104</v>
@@ -4438,7 +4432,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G66" t="s">
         <v>103</v>
@@ -4449,7 +4443,7 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C67" t="s">
         <v>106</v>
@@ -4461,7 +4455,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G67" t="s">
         <v>105</v>
@@ -4472,7 +4466,7 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C68" t="s">
         <v>108</v>
@@ -4484,7 +4478,7 @@
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G68" t="s">
         <v>107</v>
@@ -4495,7 +4489,7 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C69" t="s">
         <v>110</v>
@@ -4507,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="G69" t="s">
         <v>109</v>
@@ -4518,7 +4512,7 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C70" t="s">
         <v>112</v>
@@ -4530,7 +4524,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G70" t="s">
         <v>111</v>
@@ -4541,7 +4535,7 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C71" t="s">
         <v>100</v>
@@ -4553,7 +4547,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G71" t="s">
         <v>98</v>
@@ -4564,7 +4558,7 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C72" t="s">
         <v>99</v>
@@ -4576,7 +4570,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G72" t="s">
         <v>98</v>
@@ -4587,7 +4581,7 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C73" t="s">
         <v>101</v>
@@ -4599,7 +4593,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G73" t="s">
         <v>98</v>
@@ -4610,7 +4604,7 @@
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C74" t="s">
         <v>102</v>
@@ -4622,7 +4616,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G74" t="s">
         <v>98</v>
@@ -4633,7 +4627,7 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C75" t="s">
         <v>121</v>
@@ -4645,7 +4639,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G75" t="s">
         <v>121</v>
@@ -4656,7 +4650,7 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C76" t="s">
         <v>129</v>
@@ -4668,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G76" t="s">
         <v>129</v>
@@ -4679,7 +4673,7 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C77" t="s">
         <v>128</v>
@@ -4691,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G77" t="s">
         <v>128</v>
@@ -4702,7 +4696,7 @@
         <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C78" t="s">
         <v>125</v>
@@ -4714,7 +4708,7 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G78" t="s">
         <v>125</v>
@@ -4725,7 +4719,7 @@
         <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C79" t="s">
         <v>123</v>
@@ -4737,7 +4731,7 @@
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G79" t="s">
         <v>122</v>
@@ -4748,7 +4742,7 @@
         <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C80" t="s">
         <v>124</v>
@@ -4760,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G80" t="s">
         <v>124</v>
@@ -4771,7 +4765,7 @@
         <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C81" t="s">
         <v>118</v>
@@ -4783,10 +4777,10 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G81" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -4794,7 +4788,7 @@
         <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C82" t="s">
         <v>131</v>
@@ -4806,7 +4800,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G82" t="s">
         <v>130</v>
@@ -4817,7 +4811,7 @@
         <v>89</v>
       </c>
       <c r="B83" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C83" t="s">
         <v>118</v>
@@ -4829,7 +4823,7 @@
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G83" t="s">
         <v>117</v>
@@ -4840,10 +4834,10 @@
         <v>91</v>
       </c>
       <c r="B84" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C84" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D84" s="1">
         <v>299</v>
@@ -4852,10 +4846,10 @@
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G84" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -4863,7 +4857,7 @@
         <v>93</v>
       </c>
       <c r="B85" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C85" t="s">
         <v>120</v>
@@ -4875,7 +4869,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G85" t="s">
         <v>119</v>
@@ -4886,7 +4880,7 @@
         <v>95</v>
       </c>
       <c r="B86" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C86" t="s">
         <v>135</v>
@@ -4898,7 +4892,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G86" t="s">
         <v>135</v>
@@ -4909,10 +4903,10 @@
         <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C87" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D87" s="1">
         <v>59</v>
@@ -4921,10 +4915,10 @@
         <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G87" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -4932,7 +4926,7 @@
         <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C88" t="s">
         <v>134</v>
@@ -4944,7 +4938,7 @@
         <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G88" t="s">
         <v>134</v>
@@ -4955,7 +4949,7 @@
         <v>98</v>
       </c>
       <c r="B89" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C89" t="s">
         <v>136</v>
@@ -4967,7 +4961,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G89" t="s">
         <v>136</v>
@@ -4978,10 +4972,10 @@
         <v>99</v>
       </c>
       <c r="B90" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C90" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D90" s="1">
         <v>179</v>
@@ -4990,10 +4984,10 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G90" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -5001,7 +4995,7 @@
         <v>100</v>
       </c>
       <c r="B91" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C91" t="s">
         <v>133</v>
@@ -5013,7 +5007,7 @@
         <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>132</v>
@@ -5024,10 +5018,10 @@
         <v>101</v>
       </c>
       <c r="B92" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C92" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D92" s="1">
         <v>399</v>
@@ -5036,10 +5030,10 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G92" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -5047,7 +5041,7 @@
         <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>137</v>
@@ -5059,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>137</v>
@@ -5074,7 +5068,7 @@
         <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C94" t="s">
         <v>139</v>
@@ -5086,7 +5080,7 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>138</v>
@@ -5109,7 +5103,7 @@
         <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G95" t="s">
         <v>158</v>
@@ -5132,7 +5126,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G96" t="s">
         <v>158</v>
@@ -5155,7 +5149,7 @@
         <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G97" t="s">
         <v>158</v>
@@ -5178,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G98" t="s">
         <v>158</v>
@@ -5201,7 +5195,7 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G99" t="s">
         <v>158</v>
@@ -5224,7 +5218,7 @@
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G100" t="s">
         <v>158</v>
@@ -5247,7 +5241,7 @@
         <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G101" t="s">
         <v>141</v>
@@ -5270,7 +5264,7 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G102" t="s">
         <v>166</v>
@@ -5293,7 +5287,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G103" t="s">
         <v>153</v>
@@ -5316,7 +5310,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G104" t="s">
         <v>153</v>
@@ -5339,7 +5333,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G105" t="s">
         <v>156</v>
@@ -5362,7 +5356,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G106" t="s">
         <v>153</v>
@@ -5385,7 +5379,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G107" t="s">
         <v>143</v>
@@ -5408,7 +5402,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G108" t="s">
         <v>152</v>
@@ -5431,7 +5425,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G109" t="s">
         <v>158</v>
@@ -5445,7 +5439,7 @@
         <v>140</v>
       </c>
       <c r="C110" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D110" s="1">
         <v>9.9</v>
@@ -5454,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G110" t="s">
         <v>158</v>
@@ -5477,7 +5471,7 @@
         <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G111" t="s">
         <v>147</v>
@@ -5500,7 +5494,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G112" t="s">
         <v>145</v>
@@ -5523,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G113" t="s">
         <v>149</v>
@@ -5546,7 +5540,7 @@
         <v>1</v>
       </c>
       <c r="F114" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G114" t="s">
         <v>150</v>
@@ -5569,7 +5563,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G115" t="s">
         <v>151</v>
@@ -5583,7 +5577,7 @@
         <v>167</v>
       </c>
       <c r="C116" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D116" s="1">
         <v>9.9</v>
@@ -5592,7 +5586,7 @@
         <v>1</v>
       </c>
       <c r="F116" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G116" t="s">
         <v>168</v>
@@ -5615,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G117" t="s">
         <v>168</v>
@@ -5629,7 +5623,7 @@
         <v>167</v>
       </c>
       <c r="C118" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D118" s="1">
         <v>10</v>
@@ -5638,7 +5632,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G118" t="s">
         <v>168</v>
@@ -5661,7 +5655,7 @@
         <v>1</v>
       </c>
       <c r="F119" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G119" t="s">
         <v>168</v>
@@ -5684,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G120" t="s">
         <v>168</v>
@@ -5707,7 +5701,7 @@
         <v>1</v>
       </c>
       <c r="F121" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G121" t="s">
         <v>168</v>
@@ -5730,7 +5724,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G122" t="s">
         <v>189</v>
@@ -5753,7 +5747,7 @@
         <v>1</v>
       </c>
       <c r="F123" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G123" t="s">
         <v>168</v>
@@ -5776,7 +5770,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G124" t="s">
         <v>168</v>
@@ -5799,7 +5793,7 @@
         <v>1</v>
       </c>
       <c r="F125" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G125" t="s">
         <v>168</v>
@@ -5822,7 +5816,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G126" t="s">
         <v>178</v>
@@ -5845,7 +5839,7 @@
         <v>1</v>
       </c>
       <c r="F127" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G127" t="s">
         <v>191</v>
@@ -5868,7 +5862,7 @@
         <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G128" t="s">
         <v>168</v>
@@ -5891,7 +5885,7 @@
         <v>1</v>
       </c>
       <c r="F129" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G129" t="s">
         <v>187</v>
@@ -5914,7 +5908,7 @@
         <v>1</v>
       </c>
       <c r="F130" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G130" t="s">
         <v>168</v>
@@ -5937,7 +5931,7 @@
         <v>1</v>
       </c>
       <c r="F131" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G131" t="s">
         <v>168</v>
@@ -5960,7 +5954,7 @@
         <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G132" t="s">
         <v>183</v>
@@ -5983,7 +5977,7 @@
         <v>1</v>
       </c>
       <c r="F133" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G133" t="s">
         <v>181</v>
@@ -6006,7 +6000,7 @@
         <v>1</v>
       </c>
       <c r="F134" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G134" t="s">
         <v>181</v>
@@ -6029,7 +6023,7 @@
         <v>1</v>
       </c>
       <c r="F135" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G135" t="s">
         <v>205</v>
@@ -6040,7 +6034,7 @@
         <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C136" t="s">
         <v>201</v>
@@ -6052,7 +6046,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G136" t="s">
         <v>200</v>
@@ -6063,7 +6057,7 @@
         <v>147</v>
       </c>
       <c r="B137" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C137" t="s">
         <v>202</v>
@@ -6075,7 +6069,7 @@
         <v>1</v>
       </c>
       <c r="F137" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G137" t="s">
         <v>200</v>
@@ -6086,7 +6080,7 @@
         <v>148</v>
       </c>
       <c r="B138" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C138" t="s">
         <v>203</v>
@@ -6098,7 +6092,7 @@
         <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="G138" t="s">
         <v>200</v>
@@ -6109,7 +6103,7 @@
         <v>149</v>
       </c>
       <c r="B139" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C139" t="s">
         <v>195</v>
@@ -6121,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="F139" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G139" t="s">
         <v>194</v>
@@ -6132,7 +6126,7 @@
         <v>150</v>
       </c>
       <c r="B140" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C140" t="s">
         <v>196</v>
@@ -6144,7 +6138,7 @@
         <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G140" t="s">
         <v>194</v>
@@ -6155,7 +6149,7 @@
         <v>151</v>
       </c>
       <c r="B141" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C141" t="s">
         <v>197</v>
@@ -6167,7 +6161,7 @@
         <v>1</v>
       </c>
       <c r="F141" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="G141" t="s">
         <v>194</v>
@@ -6178,7 +6172,7 @@
         <v>152</v>
       </c>
       <c r="B142" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C142" t="s">
         <v>199</v>
@@ -6190,7 +6184,7 @@
         <v>1</v>
       </c>
       <c r="F142" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G142" t="s">
         <v>198</v>
@@ -6201,7 +6195,7 @@
         <v>153</v>
       </c>
       <c r="B143" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C143" t="s">
         <v>193</v>
@@ -6213,7 +6207,7 @@
         <v>1</v>
       </c>
       <c r="F143" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="G143" t="s">
         <v>192</v>
@@ -6236,7 +6230,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G144" t="s">
         <v>207</v>
@@ -6259,7 +6253,7 @@
         <v>1</v>
       </c>
       <c r="F145" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G145" t="s">
         <v>209</v>
@@ -6282,7 +6276,7 @@
         <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G146" t="s">
         <v>211</v>
@@ -6305,7 +6299,7 @@
         <v>1</v>
       </c>
       <c r="F147" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G147" t="s">
         <v>213</v>
@@ -6328,7 +6322,7 @@
         <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G148" t="s">
         <v>215</v>
@@ -6351,7 +6345,7 @@
         <v>1</v>
       </c>
       <c r="F149" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G149" t="s">
         <v>217</v>
@@ -6374,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="F150" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G150" t="s">
         <v>219</v>
@@ -6397,7 +6391,7 @@
         <v>1</v>
       </c>
       <c r="F151" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G151" t="s">
         <v>221</v>
@@ -6420,7 +6414,7 @@
         <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G152" t="s">
         <v>223</v>
@@ -6443,7 +6437,7 @@
         <v>1</v>
       </c>
       <c r="F153" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G153" t="s">
         <v>226</v>
@@ -6466,7 +6460,7 @@
         <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G154" t="s">
         <v>226</v>
@@ -6489,7 +6483,7 @@
         <v>1</v>
       </c>
       <c r="F155" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G155" t="s">
         <v>226</v>
@@ -6512,7 +6506,7 @@
         <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G156" t="s">
         <v>230</v>
@@ -6535,7 +6529,7 @@
         <v>1</v>
       </c>
       <c r="F157" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G157" t="s">
         <v>230</v>
@@ -6558,7 +6552,7 @@
         <v>1</v>
       </c>
       <c r="F158" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G158" t="s">
         <v>232</v>
@@ -6581,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="F159" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G159" t="s">
         <v>234</v>
@@ -6604,7 +6598,7 @@
         <v>1</v>
       </c>
       <c r="F160" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G160" t="s">
         <v>238</v>
@@ -6621,13 +6615,13 @@
         <v>240</v>
       </c>
       <c r="D161" s="4">
-        <v>501</v>
+        <v>399</v>
       </c>
       <c r="E161" s="3">
         <v>1</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G161" s="3" t="s">
         <v>238</v>
@@ -6635,30 +6629,30 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>237</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>241</v>
+        <v>347</v>
       </c>
       <c r="D162" s="4">
+        <v>399</v>
+      </c>
+      <c r="E162" s="3">
+        <v>1</v>
+      </c>
+      <c r="F162" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="E162" s="3">
-        <v>0</v>
-      </c>
-      <c r="F162" s="3" t="s">
-        <v>501</v>
-      </c>
       <c r="G162" s="3" t="s">
-        <v>238</v>
+        <v>346</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>237</v>
@@ -6667,7 +6661,7 @@
         <v>348</v>
       </c>
       <c r="D163" s="4">
-        <v>399.1</v>
+        <v>499</v>
       </c>
       <c r="E163" s="3">
         <v>1</v>
@@ -6676,12 +6670,12 @@
         <v>502</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>237</v>
@@ -6690,13 +6684,13 @@
         <v>349</v>
       </c>
       <c r="D164" s="4">
-        <v>499.1</v>
+        <v>799</v>
       </c>
       <c r="E164" s="3">
         <v>1</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>246</v>
@@ -6704,246 +6698,246 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>176</v>
+        <v>239</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>237</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>350</v>
+        <v>580</v>
       </c>
       <c r="D165" s="4">
-        <v>799.1</v>
+        <v>500</v>
       </c>
       <c r="E165" s="3">
         <v>1</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="G165" s="3" t="s">
-        <v>247</v>
+        <v>581</v>
+      </c>
+      <c r="G165" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>239</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="D166" s="4">
-        <v>500.1</v>
-      </c>
-      <c r="E166" s="3">
-        <v>1</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>583</v>
+        <v>179</v>
+      </c>
+      <c r="B166" t="s">
+        <v>575</v>
+      </c>
+      <c r="C166" t="s">
+        <v>345</v>
+      </c>
+      <c r="D166" s="1">
+        <v>499</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166" t="s">
+        <v>419</v>
       </c>
       <c r="G166" t="s">
-        <v>584</v>
+        <v>345</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B167" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C167" t="s">
-        <v>346</v>
+        <v>256</v>
       </c>
       <c r="D167" s="1">
-        <v>499</v>
+        <v>19.5</v>
       </c>
       <c r="E167">
         <v>1</v>
       </c>
       <c r="F167" t="s">
-        <v>420</v>
+        <v>506</v>
       </c>
       <c r="G167" t="s">
-        <v>346</v>
+        <v>256</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B168" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C168" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D168" s="1">
-        <v>19.5</v>
+        <v>59</v>
       </c>
       <c r="E168">
         <v>1</v>
       </c>
       <c r="F168" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G168" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B169" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C169" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="D169" s="1">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E169">
         <v>1</v>
       </c>
       <c r="F169" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G169" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B170" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C170" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D170" s="1">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="E170">
         <v>1</v>
       </c>
       <c r="F170" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G170" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B171" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C171" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="D171" s="1">
-        <v>99</v>
+        <v>229</v>
       </c>
       <c r="E171">
         <v>1</v>
       </c>
       <c r="F171" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G171" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B172" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C172" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D172" s="1">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="E172">
         <v>1</v>
       </c>
       <c r="F172" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G172" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B173" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C173" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D173" s="1">
-        <v>269</v>
+        <v>399</v>
       </c>
       <c r="E173">
         <v>1</v>
       </c>
       <c r="F173" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G173" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B174" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C174" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D174" s="1">
-        <v>399</v>
+        <v>899</v>
       </c>
       <c r="E174">
         <v>1</v>
       </c>
       <c r="F174" t="s">
-        <v>514</v>
-      </c>
-      <c r="G174" t="s">
-        <v>251</v>
+        <v>513</v>
+      </c>
+      <c r="G174" s="5" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B175" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C175" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D175" s="1">
-        <v>899</v>
+        <v>1799</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -6952,96 +6946,96 @@
         <v>515</v>
       </c>
       <c r="G175" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B176" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C176" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D176" s="1">
-        <v>1799</v>
+        <v>1599</v>
       </c>
       <c r="E176">
         <v>1</v>
       </c>
       <c r="F176" t="s">
-        <v>517</v>
-      </c>
-      <c r="G176" s="5" t="s">
-        <v>248</v>
+        <v>516</v>
+      </c>
+      <c r="G176" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B177" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C177" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="D177" s="1">
-        <v>1599</v>
+        <v>19.5</v>
       </c>
       <c r="E177">
         <v>1</v>
       </c>
       <c r="F177" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G177" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B178" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C178" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D178" s="1">
-        <v>19.5</v>
+        <v>59</v>
       </c>
       <c r="E178">
         <v>1</v>
       </c>
       <c r="F178" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G178" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B179" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C179" t="s">
         <v>266</v>
       </c>
       <c r="D179" s="1">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E179">
         <v>1</v>
       </c>
       <c r="F179" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G179" t="s">
         <v>266</v>
@@ -7049,68 +7043,68 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B180" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C180" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D180" s="1">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="E180">
         <v>1</v>
       </c>
       <c r="F180" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G180" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B181" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C181" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D181" s="1">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="E181">
         <v>1</v>
       </c>
       <c r="F181" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G181" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B182" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C182" t="s">
         <v>270</v>
       </c>
       <c r="D182" s="1">
-        <v>229</v>
+        <v>269</v>
       </c>
       <c r="E182">
         <v>1</v>
       </c>
       <c r="F182" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G182" t="s">
         <v>270</v>
@@ -7118,36 +7112,36 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B183" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C183" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D183" s="1">
-        <v>269</v>
+        <v>399</v>
       </c>
       <c r="E183">
         <v>1</v>
       </c>
       <c r="F183" t="s">
-        <v>524</v>
-      </c>
-      <c r="G183" t="s">
-        <v>271</v>
+        <v>523</v>
+      </c>
+      <c r="G183" s="5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B184" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C184" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D184" s="1">
         <v>399</v>
@@ -7156,139 +7150,139 @@
         <v>1</v>
       </c>
       <c r="F184" t="s">
-        <v>525</v>
-      </c>
-      <c r="G184" s="5" t="s">
-        <v>262</v>
+        <v>524</v>
+      </c>
+      <c r="G184" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B185" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C185" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D185" s="1">
-        <v>399</v>
+        <v>599</v>
       </c>
       <c r="E185">
         <v>1</v>
       </c>
       <c r="F185" t="s">
-        <v>526</v>
-      </c>
-      <c r="G185" t="s">
-        <v>269</v>
+        <v>525</v>
+      </c>
+      <c r="G185" s="5" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B186" t="s">
-        <v>579</v>
+        <v>276</v>
       </c>
       <c r="C186" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D186" s="1">
-        <v>599</v>
+        <v>5.2</v>
       </c>
       <c r="E186">
         <v>1</v>
       </c>
       <c r="F186" t="s">
-        <v>527</v>
-      </c>
-      <c r="G186" s="5" t="s">
-        <v>272</v>
+        <v>526</v>
+      </c>
+      <c r="G186" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B187" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C187" t="s">
+        <v>282</v>
+      </c>
+      <c r="D187" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="F187" t="s">
+        <v>526</v>
+      </c>
+      <c r="G187" t="s">
         <v>281</v>
-      </c>
-      <c r="D187" s="1">
-        <v>5.2</v>
-      </c>
-      <c r="E187">
-        <v>1</v>
-      </c>
-      <c r="F187" t="s">
-        <v>528</v>
-      </c>
-      <c r="G187" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B188" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C188" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D188" s="1">
-        <v>7.15</v>
+        <v>12.95</v>
       </c>
       <c r="E188">
         <v>1</v>
       </c>
       <c r="F188" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G188" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B189" t="s">
+        <v>276</v>
+      </c>
+      <c r="C189" t="s">
+        <v>278</v>
+      </c>
+      <c r="D189" s="1">
+        <v>16.25</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189" t="s">
+        <v>526</v>
+      </c>
+      <c r="G189" t="s">
         <v>277</v>
-      </c>
-      <c r="C189" t="s">
-        <v>286</v>
-      </c>
-      <c r="D189" s="1">
-        <v>12.95</v>
-      </c>
-      <c r="E189">
-        <v>1</v>
-      </c>
-      <c r="F189" t="s">
-        <v>529</v>
-      </c>
-      <c r="G189" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B190" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C190" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D190" s="1">
-        <v>16.25</v>
+        <v>25</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -7297,292 +7291,292 @@
         <v>528</v>
       </c>
       <c r="G190" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B191" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="C191" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D191" s="1">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E191">
         <v>1</v>
       </c>
       <c r="F191" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G191" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B192" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C192" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D192" s="1">
-        <v>100</v>
+        <v>3.9</v>
       </c>
       <c r="E192">
         <v>1</v>
       </c>
       <c r="F192" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G192" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B193" t="s">
+        <v>289</v>
+      </c>
+      <c r="C193" t="s">
+        <v>292</v>
+      </c>
+      <c r="D193" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="E193">
+        <v>1</v>
+      </c>
+      <c r="F193" t="s">
+        <v>531</v>
+      </c>
+      <c r="G193" t="s">
         <v>290</v>
-      </c>
-      <c r="C193" t="s">
-        <v>294</v>
-      </c>
-      <c r="D193" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="E193">
-        <v>1</v>
-      </c>
-      <c r="F193" t="s">
-        <v>532</v>
-      </c>
-      <c r="G193" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B194" t="s">
+        <v>289</v>
+      </c>
+      <c r="C194" t="s">
+        <v>291</v>
+      </c>
+      <c r="D194" s="1">
+        <v>39</v>
+      </c>
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194" t="s">
+        <v>532</v>
+      </c>
+      <c r="G194" t="s">
         <v>290</v>
-      </c>
-      <c r="C194" t="s">
-        <v>293</v>
-      </c>
-      <c r="D194" s="1">
-        <v>6.9</v>
-      </c>
-      <c r="E194">
-        <v>1</v>
-      </c>
-      <c r="F194" t="s">
-        <v>533</v>
-      </c>
-      <c r="G194" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B195" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C195" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D195" s="1">
-        <v>39</v>
+        <v>39.9</v>
       </c>
       <c r="E195">
         <v>1</v>
       </c>
       <c r="F195" t="s">
-        <v>534</v>
-      </c>
-      <c r="G195" t="s">
-        <v>291</v>
+        <v>533</v>
+      </c>
+      <c r="G195" s="5" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B196" t="s">
-        <v>290</v>
+        <v>565</v>
       </c>
       <c r="C196" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D196" s="1">
-        <v>39.9</v>
+        <v>7</v>
       </c>
       <c r="E196">
         <v>1</v>
       </c>
       <c r="F196" t="s">
-        <v>535</v>
-      </c>
-      <c r="G196" s="5" t="s">
-        <v>295</v>
+        <v>534</v>
+      </c>
+      <c r="G196" t="s">
+        <v>298</v>
+      </c>
+      <c r="H196" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B197" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C197" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D197" s="1">
-        <v>7</v>
+        <v>12.9</v>
       </c>
       <c r="E197">
         <v>1</v>
       </c>
       <c r="F197" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G197" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H197" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B198" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C198" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D198" s="1">
-        <v>12.9</v>
+        <v>34.5</v>
       </c>
       <c r="E198">
         <v>1</v>
       </c>
       <c r="F198" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G198" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H198" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B199" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C199" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D199" s="1">
-        <v>34.5</v>
+        <v>99</v>
       </c>
       <c r="E199">
         <v>1</v>
       </c>
       <c r="F199" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G199" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H199" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B200" t="s">
-        <v>567</v>
+        <v>300</v>
       </c>
       <c r="C200" t="s">
-        <v>297</v>
+        <v>338</v>
       </c>
       <c r="D200" s="1">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="E200">
         <v>1</v>
       </c>
       <c r="F200" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G200" t="s">
-        <v>297</v>
-      </c>
-      <c r="H200" t="s">
-        <v>593</v>
+        <v>338</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B201" t="s">
+        <v>300</v>
+      </c>
+      <c r="C201" t="s">
         <v>301</v>
       </c>
-      <c r="C201" t="s">
-        <v>339</v>
-      </c>
       <c r="D201" s="1">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E201">
         <v>1</v>
       </c>
       <c r="F201" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G201" t="s">
-        <v>339</v>
+        <v>301</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B202" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C202" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D202" s="1">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="E202">
         <v>1</v>
       </c>
       <c r="F202" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G202" t="s">
         <v>302</v>
@@ -7590,16 +7584,16 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B203" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C203" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D203" s="1">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -7608,15 +7602,15 @@
         <v>542</v>
       </c>
       <c r="G203" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B204" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C204" t="s">
         <v>308</v>
@@ -7628,7 +7622,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G204" t="s">
         <v>308</v>
@@ -7636,10 +7630,10 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B205" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C205" t="s">
         <v>309</v>
@@ -7651,7 +7645,7 @@
         <v>1</v>
       </c>
       <c r="F205" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G205" t="s">
         <v>309</v>
@@ -7659,10 +7653,10 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B206" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C206" t="s">
         <v>310</v>
@@ -7674,7 +7668,7 @@
         <v>1</v>
       </c>
       <c r="F206" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G206" t="s">
         <v>310</v>
@@ -7682,10 +7676,10 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B207" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C207" t="s">
         <v>311</v>
@@ -7697,7 +7691,7 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G207" t="s">
         <v>311</v>
@@ -7705,33 +7699,33 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B208" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C208" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D208" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E208">
         <v>1</v>
       </c>
       <c r="F208" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G208" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B209" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C209" t="s">
         <v>315</v>
@@ -7743,18 +7737,18 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G209" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B210" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C210" t="s">
         <v>316</v>
@@ -7766,18 +7760,18 @@
         <v>1</v>
       </c>
       <c r="F210" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G210" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C211" t="s">
         <v>317</v>
@@ -7789,41 +7783,41 @@
         <v>1</v>
       </c>
       <c r="F211" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G211" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B212" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C212" t="s">
+        <v>319</v>
+      </c>
+      <c r="D212" s="1">
+        <v>6</v>
+      </c>
+      <c r="E212">
+        <v>1</v>
+      </c>
+      <c r="F212" t="s">
+        <v>548</v>
+      </c>
+      <c r="G212" t="s">
         <v>318</v>
-      </c>
-      <c r="D212" s="1">
-        <v>19</v>
-      </c>
-      <c r="E212">
-        <v>1</v>
-      </c>
-      <c r="F212" t="s">
-        <v>549</v>
-      </c>
-      <c r="G212" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B213" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C213" t="s">
         <v>320</v>
@@ -7835,41 +7829,41 @@
         <v>1</v>
       </c>
       <c r="F213" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G213" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B214" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C214" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D214" s="1">
-        <v>6</v>
+        <v>9.9</v>
       </c>
       <c r="E214">
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G214" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B215" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C215" t="s">
         <v>324</v>
@@ -7881,21 +7875,21 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G215" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B216" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C216" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D216" s="1">
         <v>9.9</v>
@@ -7904,18 +7898,18 @@
         <v>1</v>
       </c>
       <c r="F216" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G216" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B217" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C217" t="s">
         <v>327</v>
@@ -7927,67 +7921,67 @@
         <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G217" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B218" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C218" t="s">
+        <v>329</v>
+      </c>
+      <c r="D218" s="1">
+        <v>12</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218" t="s">
+        <v>554</v>
+      </c>
+      <c r="G218" t="s">
         <v>328</v>
-      </c>
-      <c r="D218" s="1">
-        <v>9.9</v>
-      </c>
-      <c r="E218">
-        <v>1</v>
-      </c>
-      <c r="F218" t="s">
-        <v>555</v>
-      </c>
-      <c r="G218" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B219" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C219" t="s">
+        <v>331</v>
+      </c>
+      <c r="D219" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+      <c r="F219" t="s">
+        <v>555</v>
+      </c>
+      <c r="G219" t="s">
         <v>330</v>
-      </c>
-      <c r="D219" s="1">
-        <v>12</v>
-      </c>
-      <c r="E219">
-        <v>1</v>
-      </c>
-      <c r="F219" t="s">
-        <v>556</v>
-      </c>
-      <c r="G219" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B220" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C220" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D220" s="1">
         <v>18.899999999999999</v>
@@ -7996,425 +7990,425 @@
         <v>1</v>
       </c>
       <c r="F220" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G220" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="B221" t="s">
-        <v>322</v>
+        <v>592</v>
       </c>
       <c r="C221" t="s">
-        <v>334</v>
+        <v>596</v>
       </c>
       <c r="D221" s="1">
-        <v>18.899999999999999</v>
+        <v>14800</v>
       </c>
       <c r="E221">
         <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>558</v>
+        <v>597</v>
       </c>
       <c r="G221" t="s">
-        <v>333</v>
+        <v>598</v>
+      </c>
+      <c r="H221" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B222" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C222" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D222" s="1">
-        <v>14800</v>
+        <v>580</v>
       </c>
       <c r="E222">
         <v>1</v>
       </c>
       <c r="F222" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="G222" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="H222" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B223" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C223" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D223" s="1">
-        <v>580</v>
+        <v>3800</v>
       </c>
       <c r="E223">
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="G223" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="H223" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B224" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C224" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="D224" s="1">
-        <v>3800</v>
+        <v>6800</v>
       </c>
       <c r="E224">
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="G224" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H224" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B225" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C225" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D225" s="1">
-        <v>6800</v>
+        <v>599</v>
       </c>
       <c r="E225">
         <v>1</v>
       </c>
       <c r="F225" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G225" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H225" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B226" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C226" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D226" s="1">
-        <v>599</v>
+        <v>799</v>
       </c>
       <c r="E226">
         <v>1</v>
       </c>
       <c r="F226" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G226" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="H226" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B227" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C227" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D227" s="1">
-        <v>799</v>
+        <v>1700</v>
       </c>
       <c r="E227">
         <v>1</v>
       </c>
       <c r="F227" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="G227" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="H227" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B228" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C228" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="D228" s="1">
-        <v>1700</v>
+        <v>1990</v>
       </c>
       <c r="E228">
         <v>1</v>
       </c>
       <c r="F228" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="G228" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="H228" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B229" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C229" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D229" s="1">
-        <v>1990</v>
+        <v>2999</v>
       </c>
       <c r="E229">
         <v>1</v>
       </c>
       <c r="F229" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="G229" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H229" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B230" t="s">
-        <v>594</v>
+        <v>629</v>
       </c>
       <c r="C230" t="s">
-        <v>628</v>
+        <v>596</v>
       </c>
       <c r="D230" s="1">
-        <v>2999</v>
+        <v>1400</v>
       </c>
       <c r="E230">
         <v>1</v>
       </c>
       <c r="F230" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="G230" t="s">
-        <v>630</v>
-      </c>
-      <c r="H230" t="s">
-        <v>669</v>
+        <v>631</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B231" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C231" t="s">
-        <v>598</v>
+        <v>632</v>
       </c>
       <c r="D231" s="1">
-        <v>1400</v>
+        <v>999</v>
       </c>
       <c r="E231">
         <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="G231" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B232" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C232" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D232" s="1">
-        <v>999</v>
+        <v>1500</v>
       </c>
       <c r="E232">
         <v>1</v>
       </c>
       <c r="F232" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="G232" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B233" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C233" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D233" s="1">
-        <v>1500</v>
+        <v>1299</v>
       </c>
       <c r="E233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F233" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G233" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B234" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C234" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D234" s="1">
-        <v>1299</v>
+        <v>799</v>
       </c>
       <c r="E234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F234" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="G234" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B235" t="s">
-        <v>631</v>
+        <v>27</v>
       </c>
       <c r="C235" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D235" s="1">
-        <v>799</v>
+        <v>849</v>
       </c>
       <c r="E235">
         <v>1</v>
       </c>
       <c r="F235" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="G235" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B236" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C236" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D236" s="1">
-        <v>849</v>
+        <v>450</v>
       </c>
       <c r="E236">
         <v>1</v>
       </c>
       <c r="F236" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="G236" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B237" t="s">
-        <v>37</v>
+        <v>578</v>
       </c>
       <c r="C237" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D237" s="1">
-        <v>450</v>
+        <v>699</v>
       </c>
       <c r="E237">
         <v>1</v>
       </c>
       <c r="F237" t="s">
-        <v>650</v>
+        <v>668</v>
       </c>
       <c r="G237" t="s">
         <v>651</v>
@@ -8422,128 +8416,105 @@
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B238" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C238" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="D238" s="1">
-        <v>699</v>
+        <v>999</v>
       </c>
       <c r="E238">
         <v>1</v>
       </c>
       <c r="F238" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
       <c r="G238" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B239" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="C239" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D239" s="1">
-        <v>999</v>
+        <v>599</v>
       </c>
       <c r="E239">
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="G239" t="s">
-        <v>659</v>
+        <v>660</v>
+      </c>
+      <c r="H239" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B240" t="s">
-        <v>594</v>
+        <v>62</v>
       </c>
       <c r="C240" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D240" s="1">
-        <v>599</v>
+        <v>1100</v>
       </c>
       <c r="E240">
         <v>1</v>
       </c>
       <c r="F240" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="G240" t="s">
-        <v>662</v>
-      </c>
-      <c r="H240" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B241" t="s">
-        <v>62</v>
+        <v>579</v>
       </c>
       <c r="C241" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D241" s="1">
-        <v>1100</v>
+        <v>1999</v>
       </c>
       <c r="E241">
         <v>1</v>
       </c>
       <c r="F241" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="G241" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A242">
-        <v>274</v>
-      </c>
-      <c r="B242" t="s">
-        <v>581</v>
-      </c>
-      <c r="C242" t="s">
         <v>666</v>
       </c>
-      <c r="D242" s="1">
-        <v>1999</v>
-      </c>
-      <c r="E242">
-        <v>1</v>
-      </c>
-      <c r="F242" t="s">
-        <v>667</v>
-      </c>
-      <c r="G242" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D244" s="1"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D243" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A201:G203">
-    <sortCondition ref="D201:D203"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A200:G202">
+    <sortCondition ref="D200:D202"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8572,7 +8543,7 @@
         <v>237</v>
       </c>
       <c r="C1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D1" s="1">
         <v>999</v>
@@ -8581,10 +8552,10 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -8595,7 +8566,7 @@
         <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D2" s="1">
         <v>999</v>
@@ -8604,10 +8575,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8618,7 +8589,7 @@
         <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D3" s="1">
         <v>499</v>
@@ -8627,10 +8598,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8641,7 +8612,7 @@
         <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D4" s="1">
         <v>599</v>
@@ -8650,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G4" t="s">
         <v>85</v>
@@ -8673,7 +8644,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G5" t="s">
         <v>63</v>
@@ -8696,7 +8667,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G6" t="s">
         <v>77</v>
@@ -8719,7 +8690,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G7" t="s">
         <v>90</v>
@@ -8730,10 +8701,10 @@
         <v>220</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D8" s="1">
         <v>399</v>
@@ -8742,10 +8713,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -8753,10 +8724,10 @@
         <v>259</v>
       </c>
       <c r="B9" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C9" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D9" s="1">
         <v>9800</v>
@@ -8765,13 +8736,13 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G9" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H9" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -8779,7 +8750,7 @@
         <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C10" t="s">
         <v>127</v>
@@ -8791,7 +8762,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G10" t="s">
         <v>126</v>
@@ -8802,10 +8773,10 @@
         <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D11" s="1">
         <v>1299</v>
@@ -8814,10 +8785,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="G11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -8825,10 +8796,10 @@
         <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="1">
         <v>1299</v>
@@ -8837,10 +8808,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -8860,7 +8831,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G13" t="s">
         <v>56</v>
@@ -8871,10 +8842,10 @@
         <v>250</v>
       </c>
       <c r="B14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D14" s="1">
         <v>7800</v>
@@ -8883,13 +8854,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="G14" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H14" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -8897,10 +8868,10 @@
         <v>254</v>
       </c>
       <c r="B15" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C15" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D15" s="1">
         <v>29800</v>
@@ -8909,13 +8880,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="G15" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H15" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -8923,10 +8894,10 @@
         <v>270</v>
       </c>
       <c r="B16" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C16" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D16" s="1">
         <v>1090</v>
@@ -8935,10 +8906,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G16" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -8949,7 +8920,7 @@
         <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D17" s="1">
         <v>1000</v>
@@ -8958,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G17" s="6"/>
     </row>
@@ -8970,7 +8941,7 @@
         <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D18" s="4">
         <v>399</v>
@@ -8979,7 +8950,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>75</v>
@@ -8993,7 +8964,7 @@
         <v>237</v>
       </c>
       <c r="C19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D19" s="1">
         <v>999</v>
@@ -9002,10 +8973,10 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preis geändert und Text geändert
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D400B13E-AEC0-4429-BD66-E232B49C08DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B115B-4E28-42A8-8D44-FA69DDA352F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2929,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6592,7 +6592,7 @@
         <v>239</v>
       </c>
       <c r="D160" s="1">
-        <v>450.2</v>
+        <v>399</v>
       </c>
       <c r="E160">
         <v>1</v>

</xml_diff>

<commit_message>
Produkt auf 5x erhöht
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Cintamani\Website 2017\react-cintamani\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88B115B-4E28-42A8-8D44-FA69DDA352F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C08D4E-02F3-4711-9C09-4681F1771F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2930,7 +2930,7 @@
   <dimension ref="A1:K243"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6641,7 +6641,7 @@
         <v>399</v>
       </c>
       <c r="E162" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>500</v>

</xml_diff>